<commit_message>
Site rebuild Fri Dec  6 17:10:47 CST 2019
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchattopadhyay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchattopadhyay/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3247FBB-33C0-FD45-B01D-ABAB93E53914}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D44A8A0-7015-A448-A5CC-F4C03BC3184A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{26E92A9D-7BD1-914F-959E-FC63F09E2183}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$46</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="115">
   <si>
     <t>website</t>
   </si>
@@ -373,6 +373,12 @@
   </si>
   <si>
     <t>https://www.linkedin.com/pulse/basics-python-tkinter-rajarshi-chattopadhyay</t>
+  </si>
+  <si>
+    <t>text2number</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/text2number</t>
   </si>
 </sst>
 </file>
@@ -743,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2CE227-055B-2D42-8D36-FD50B0BC9862}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1003,11 +1009,11 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>501</v>
+      <c r="B12" s="3">
+        <v>402</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="D12" t="s">
         <v>91</v>
@@ -1016,41 +1022,41 @@
         <v>95</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <v>502</v>
+      <c r="B13">
+        <v>501</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" t="s">
         <v>95</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>503</v>
+      <c r="B14" s="3">
+        <v>502</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
@@ -1059,7 +1065,7 @@
         <v>95</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1067,10 +1073,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
         <v>92</v>
@@ -1079,18 +1085,18 @@
         <v>95</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
-        <v>505</v>
+      <c r="B16">
+        <v>504</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
         <v>92</v>
@@ -1099,18 +1105,18 @@
         <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>506</v>
+      <c r="B17" s="3">
+        <v>505</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
         <v>92</v>
@@ -1119,7 +1125,7 @@
         <v>95</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1127,19 +1133,19 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E18" t="s">
         <v>95</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1147,10 +1153,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
         <v>91</v>
@@ -1159,7 +1165,7 @@
         <v>95</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1167,19 +1173,19 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
         <v>95</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1187,10 +1193,10 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>601</v>
+        <v>509</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
         <v>92</v>
@@ -1199,7 +1205,7 @@
         <v>95</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1207,10 +1213,10 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
         <v>92</v>
@@ -1219,7 +1225,7 @@
         <v>95</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1227,10 +1233,10 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
         <v>92</v>
@@ -1239,7 +1245,7 @@
         <v>95</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1247,10 +1253,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
         <v>92</v>
@@ -1259,27 +1265,27 @@
         <v>95</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
-        <v>605</v>
+      <c r="B25">
+        <v>604</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s">
         <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1287,10 +1293,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
         <v>91</v>
@@ -1299,10 +1305,7 @@
         <v>95</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1310,10 +1313,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="3">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
         <v>91</v>
@@ -1322,10 +1325,10 @@
         <v>95</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1333,10 +1336,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="3">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
         <v>91</v>
@@ -1345,7 +1348,10 @@
         <v>95</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1353,19 +1359,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="3">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E29" t="s">
         <v>95</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1373,10 +1379,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D30" t="s">
         <v>92</v>
@@ -1385,41 +1391,38 @@
         <v>95</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31">
-        <v>701</v>
+      <c r="B31" s="3">
+        <v>610</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E31" t="s">
         <v>95</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
-        <v>702</v>
+      <c r="B32">
+        <v>701</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
         <v>91</v>
@@ -1428,27 +1431,30 @@
         <v>95</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33">
-        <v>703</v>
+      <c r="B33" s="3">
+        <v>702</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E33" t="s">
         <v>95</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1456,10 +1462,10 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D34" t="s">
         <v>93</v>
@@ -1468,7 +1474,7 @@
         <v>95</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1476,19 +1482,19 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E35" t="s">
-        <v>103</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1496,10 +1502,10 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D36" t="s">
         <v>91</v>
@@ -1508,7 +1514,7 @@
         <v>103</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1516,22 +1522,19 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>801</v>
+        <v>706</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="D37" t="s">
         <v>91</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1539,31 +1542,33 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
       <c r="D38" t="s">
         <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>103</v>
-      </c>
-      <c r="F38" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G38" s="1" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="3">
-        <v>803</v>
+      <c r="B39">
+        <v>802</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D39" t="s">
         <v>91</v>
@@ -1571,28 +1576,29 @@
       <c r="E39" t="s">
         <v>103</v>
       </c>
+      <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40">
-        <v>804</v>
+      <c r="B40" s="3">
+        <v>803</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E40" t="s">
         <v>103</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1603,16 +1609,16 @@
         <v>804</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E41" t="s">
         <v>103</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1620,19 +1626,19 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C42" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="D42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E42" t="s">
-        <v>95</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>72</v>
+        <v>103</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1640,19 +1646,19 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>901</v>
+        <v>805</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="D43" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E43" t="s">
-        <v>103</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1660,22 +1666,19 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D44" t="s">
         <v>91</v>
       </c>
       <c r="E44" t="s">
-        <v>95</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1683,90 +1686,114 @@
         <v>44</v>
       </c>
       <c r="B45">
+        <v>902</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" t="s">
+        <v>91</v>
+      </c>
+      <c r="E45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
         <v>903</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>34</v>
       </c>
-      <c r="D45" t="s">
-        <v>91</v>
-      </c>
-      <c r="E45" t="s">
-        <v>95</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="D46" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" t="s">
+        <v>95</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G45" xr:uid="{27AC6761-2437-C441-907E-B1FB733C8BAA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G45">
+  <autoFilter ref="B1:G46" xr:uid="{27AC6761-2437-C441-907E-B1FB733C8BAA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G46">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G46">
     <sortCondition ref="B1"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{E26AB3C4-29AE-204B-97A1-8F7175E3530D}"/>
-    <hyperlink ref="F12" r:id="rId2" xr:uid="{20C7D150-9462-1F41-AAB7-2A899F9C969A}"/>
+    <hyperlink ref="F13" r:id="rId2" xr:uid="{20C7D150-9462-1F41-AAB7-2A899F9C969A}"/>
     <hyperlink ref="F5" r:id="rId3" xr:uid="{62DFB431-E49A-4741-B60E-DA27CFC68C72}"/>
-    <hyperlink ref="F13" r:id="rId4" xr:uid="{8506591B-A62F-6948-8F5E-FAB4DE06D345}"/>
-    <hyperlink ref="F18" r:id="rId5" xr:uid="{7B4333D3-C25D-3144-87C0-B86DA456F7A0}"/>
-    <hyperlink ref="F19" r:id="rId6" xr:uid="{6F8B3503-4C3A-DC40-8109-C9D396669308}"/>
+    <hyperlink ref="F14" r:id="rId4" xr:uid="{8506591B-A62F-6948-8F5E-FAB4DE06D345}"/>
+    <hyperlink ref="F19" r:id="rId5" xr:uid="{7B4333D3-C25D-3144-87C0-B86DA456F7A0}"/>
+    <hyperlink ref="F20" r:id="rId6" xr:uid="{6F8B3503-4C3A-DC40-8109-C9D396669308}"/>
     <hyperlink ref="F6" r:id="rId7" xr:uid="{E11F3A2B-4236-C240-B3A5-B3577F908F63}"/>
-    <hyperlink ref="F21" r:id="rId8" xr:uid="{208F8125-58C4-4848-9C44-457B5CA9C713}"/>
-    <hyperlink ref="F26" r:id="rId9" xr:uid="{3F4F2A3A-2C07-1A42-AC3D-471388B48825}"/>
-    <hyperlink ref="F27" r:id="rId10" xr:uid="{119BF651-F8C7-C24B-BA6B-34B978975A37}"/>
-    <hyperlink ref="F31" r:id="rId11" xr:uid="{2CCAB83E-F41F-B24B-90B4-A0DB21E63EAC}"/>
-    <hyperlink ref="F37" r:id="rId12" xr:uid="{0826D0C0-8E81-C044-9D15-BC27CA346E4D}"/>
-    <hyperlink ref="F30" r:id="rId13" xr:uid="{4DDE0179-60BD-8D4F-9D6C-2A707E2A6ABF}"/>
+    <hyperlink ref="F22" r:id="rId8" xr:uid="{208F8125-58C4-4848-9C44-457B5CA9C713}"/>
+    <hyperlink ref="F27" r:id="rId9" xr:uid="{3F4F2A3A-2C07-1A42-AC3D-471388B48825}"/>
+    <hyperlink ref="F28" r:id="rId10" xr:uid="{119BF651-F8C7-C24B-BA6B-34B978975A37}"/>
+    <hyperlink ref="F32" r:id="rId11" xr:uid="{2CCAB83E-F41F-B24B-90B4-A0DB21E63EAC}"/>
+    <hyperlink ref="F38" r:id="rId12" xr:uid="{0826D0C0-8E81-C044-9D15-BC27CA346E4D}"/>
+    <hyperlink ref="F31" r:id="rId13" xr:uid="{4DDE0179-60BD-8D4F-9D6C-2A707E2A6ABF}"/>
     <hyperlink ref="F7" r:id="rId14" xr:uid="{0317F90B-9CF5-D440-98C2-9DD3D8CD4360}"/>
-    <hyperlink ref="F24" r:id="rId15" xr:uid="{B0FDC84E-194C-CA4A-B974-8821AB0DA033}"/>
-    <hyperlink ref="F17" r:id="rId16" xr:uid="{5C69EB99-4BB2-6C40-B120-40DC6CEA8E3D}"/>
+    <hyperlink ref="F25" r:id="rId15" xr:uid="{B0FDC84E-194C-CA4A-B974-8821AB0DA033}"/>
+    <hyperlink ref="F18" r:id="rId16" xr:uid="{5C69EB99-4BB2-6C40-B120-40DC6CEA8E3D}"/>
     <hyperlink ref="F2" r:id="rId17" xr:uid="{F9CDDCEB-59CD-AE47-A149-9CC74B550FEC}"/>
     <hyperlink ref="F3" r:id="rId18" xr:uid="{DE3B3CAA-EE98-3047-8B1C-3EEDFEAD7F28}"/>
     <hyperlink ref="F4" r:id="rId19" xr:uid="{3C4A7730-5B0F-F648-B13F-492DD0C989D9}"/>
-    <hyperlink ref="F16" r:id="rId20" xr:uid="{C1E695B0-BCA2-C543-ACE5-568C9F0303B1}"/>
-    <hyperlink ref="F28" r:id="rId21" xr:uid="{69EB5850-A79D-2249-8859-15359590B6A7}"/>
-    <hyperlink ref="F23" r:id="rId22" xr:uid="{C61A74F0-4B76-0C4E-BB52-AC63D005FD62}"/>
-    <hyperlink ref="F22" r:id="rId23" xr:uid="{81A92251-C09C-E44E-9A36-C9FE15E5FCD8}"/>
-    <hyperlink ref="F29" r:id="rId24" xr:uid="{F4F55930-9ED7-EA4F-BCBD-BCFEE7610B82}"/>
-    <hyperlink ref="F20" r:id="rId25" xr:uid="{0091B4FD-E7C4-1B4D-9203-8698BC24D565}"/>
-    <hyperlink ref="F32" r:id="rId26" xr:uid="{EB6B87D1-21E1-FC4E-B405-2E1E5231BF06}"/>
+    <hyperlink ref="F17" r:id="rId20" xr:uid="{C1E695B0-BCA2-C543-ACE5-568C9F0303B1}"/>
+    <hyperlink ref="F29" r:id="rId21" xr:uid="{69EB5850-A79D-2249-8859-15359590B6A7}"/>
+    <hyperlink ref="F24" r:id="rId22" xr:uid="{C61A74F0-4B76-0C4E-BB52-AC63D005FD62}"/>
+    <hyperlink ref="F23" r:id="rId23" xr:uid="{81A92251-C09C-E44E-9A36-C9FE15E5FCD8}"/>
+    <hyperlink ref="F30" r:id="rId24" xr:uid="{F4F55930-9ED7-EA4F-BCBD-BCFEE7610B82}"/>
+    <hyperlink ref="F21" r:id="rId25" xr:uid="{0091B4FD-E7C4-1B4D-9203-8698BC24D565}"/>
+    <hyperlink ref="F33" r:id="rId26" xr:uid="{EB6B87D1-21E1-FC4E-B405-2E1E5231BF06}"/>
     <hyperlink ref="F11" r:id="rId27" xr:uid="{71F90D41-9C86-E340-936E-3BB9C8F90010}"/>
-    <hyperlink ref="F14" r:id="rId28" xr:uid="{3DB60B42-7507-6C4E-BDAE-4CFDF2EB9C4B}"/>
-    <hyperlink ref="F25" r:id="rId29" xr:uid="{DE0DD6CB-D570-6945-B428-B9331B5F7EBD}"/>
-    <hyperlink ref="F15" r:id="rId30" xr:uid="{FEFB8575-764E-9449-AA25-D9D9E8089739}"/>
+    <hyperlink ref="F15" r:id="rId28" xr:uid="{3DB60B42-7507-6C4E-BDAE-4CFDF2EB9C4B}"/>
+    <hyperlink ref="F26" r:id="rId29" xr:uid="{DE0DD6CB-D570-6945-B428-B9331B5F7EBD}"/>
+    <hyperlink ref="F16" r:id="rId30" xr:uid="{FEFB8575-764E-9449-AA25-D9D9E8089739}"/>
     <hyperlink ref="F9" r:id="rId31" xr:uid="{D26F3756-D827-C34C-94BF-A5B4EB60366B}"/>
     <hyperlink ref="F10" r:id="rId32" xr:uid="{784A9FC5-FAB0-B844-BE6A-3AF588A130C9}"/>
-    <hyperlink ref="F42" r:id="rId33" xr:uid="{EB6D586F-57BF-DD4A-8A35-36111ACF2E34}"/>
-    <hyperlink ref="F44" r:id="rId34" xr:uid="{4FE78F82-E051-BD41-AF8D-290EBCE2FD87}"/>
-    <hyperlink ref="F45" r:id="rId35" xr:uid="{EFC9C5A7-AB7E-6445-B238-3F6B90ECD054}"/>
-    <hyperlink ref="F33" r:id="rId36" xr:uid="{63617CDE-2E2D-AD4B-A08D-0848E898DD47}"/>
-    <hyperlink ref="F34" r:id="rId37" xr:uid="{3F4D27CA-6390-D84B-B25B-184101CE06FA}"/>
+    <hyperlink ref="F43" r:id="rId33" xr:uid="{EB6D586F-57BF-DD4A-8A35-36111ACF2E34}"/>
+    <hyperlink ref="F45" r:id="rId34" xr:uid="{4FE78F82-E051-BD41-AF8D-290EBCE2FD87}"/>
+    <hyperlink ref="F46" r:id="rId35" xr:uid="{EFC9C5A7-AB7E-6445-B238-3F6B90ECD054}"/>
+    <hyperlink ref="F34" r:id="rId36" xr:uid="{63617CDE-2E2D-AD4B-A08D-0848E898DD47}"/>
+    <hyperlink ref="F35" r:id="rId37" xr:uid="{3F4D27CA-6390-D84B-B25B-184101CE06FA}"/>
     <hyperlink ref="G8" r:id="rId38" xr:uid="{07E7E11C-8841-7748-BFFF-540D5BB62B39}"/>
-    <hyperlink ref="G12" r:id="rId39" xr:uid="{41C80DDC-B435-E44A-B9FF-4AF4DE2F5656}"/>
+    <hyperlink ref="G13" r:id="rId39" xr:uid="{41C80DDC-B435-E44A-B9FF-4AF4DE2F5656}"/>
     <hyperlink ref="G6" r:id="rId40" xr:uid="{9F0DCD01-87D0-6A40-AE3F-32FC101B7188}"/>
-    <hyperlink ref="G26" r:id="rId41" xr:uid="{197BB746-FF15-2148-98BE-5BB0F1F85567}"/>
-    <hyperlink ref="G27" r:id="rId42" xr:uid="{C77A6773-BBA6-584C-8DAC-DE08233409B2}"/>
-    <hyperlink ref="G31" r:id="rId43" xr:uid="{7FC8D046-4E44-AD48-B3AC-C616091F1C3A}"/>
-    <hyperlink ref="G37" r:id="rId44" xr:uid="{F25E562D-AAF9-4041-B937-A59BAFE18EC5}"/>
+    <hyperlink ref="G27" r:id="rId41" xr:uid="{197BB746-FF15-2148-98BE-5BB0F1F85567}"/>
+    <hyperlink ref="G28" r:id="rId42" xr:uid="{C77A6773-BBA6-584C-8DAC-DE08233409B2}"/>
+    <hyperlink ref="G32" r:id="rId43" xr:uid="{7FC8D046-4E44-AD48-B3AC-C616091F1C3A}"/>
+    <hyperlink ref="G38" r:id="rId44" xr:uid="{F25E562D-AAF9-4041-B937-A59BAFE18EC5}"/>
     <hyperlink ref="G7" r:id="rId45" xr:uid="{B3DC7E65-8B74-914F-93A8-6005B22982A3}"/>
     <hyperlink ref="G2" r:id="rId46" xr:uid="{843CA431-F6E9-1B4D-845E-601D7EDB0BB1}"/>
     <hyperlink ref="G3" r:id="rId47" xr:uid="{4D5CA3E4-8FD4-DE4A-83B2-0E8DDA142970}"/>
     <hyperlink ref="G4" r:id="rId48" xr:uid="{F45701A4-E062-F544-AEFE-3543E8569B6E}"/>
-    <hyperlink ref="G44" r:id="rId49" xr:uid="{985334CD-1972-8442-AD5A-14F3D57E92CF}"/>
-    <hyperlink ref="G45" r:id="rId50" xr:uid="{5556EC84-5DAB-B246-9C73-76642D572382}"/>
-    <hyperlink ref="G43" r:id="rId51" xr:uid="{51C1EF83-209F-024C-B3DA-10B36D1E5A4C}"/>
-    <hyperlink ref="G36" r:id="rId52" xr:uid="{BED6B18A-333C-D348-9DA2-FBE4265E3C32}"/>
-    <hyperlink ref="G35" r:id="rId53" xr:uid="{68C79AD3-9ED9-684B-BA88-B3D3EE552B52}"/>
-    <hyperlink ref="G41" r:id="rId54" xr:uid="{149FC972-472B-6F48-BC30-B43708381DDC}"/>
-    <hyperlink ref="G40" r:id="rId55" xr:uid="{6E323EF5-0E5A-5B4C-BD17-16A6D0E2C053}"/>
-    <hyperlink ref="G39" r:id="rId56" xr:uid="{96FE3BD0-D39E-7A4F-953E-7831D516D31B}"/>
+    <hyperlink ref="G45" r:id="rId49" xr:uid="{985334CD-1972-8442-AD5A-14F3D57E92CF}"/>
+    <hyperlink ref="G46" r:id="rId50" xr:uid="{5556EC84-5DAB-B246-9C73-76642D572382}"/>
+    <hyperlink ref="G44" r:id="rId51" xr:uid="{51C1EF83-209F-024C-B3DA-10B36D1E5A4C}"/>
+    <hyperlink ref="G37" r:id="rId52" xr:uid="{BED6B18A-333C-D348-9DA2-FBE4265E3C32}"/>
+    <hyperlink ref="G36" r:id="rId53" xr:uid="{68C79AD3-9ED9-684B-BA88-B3D3EE552B52}"/>
+    <hyperlink ref="G42" r:id="rId54" xr:uid="{149FC972-472B-6F48-BC30-B43708381DDC}"/>
+    <hyperlink ref="G41" r:id="rId55" xr:uid="{6E323EF5-0E5A-5B4C-BD17-16A6D0E2C053}"/>
+    <hyperlink ref="G40" r:id="rId56" xr:uid="{96FE3BD0-D39E-7A4F-953E-7831D516D31B}"/>
+    <hyperlink ref="F12" r:id="rId57" xr:uid="{D6022A27-41D7-5246-8EF9-8E2A4D9AC1A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Site rebuild Wed Dec 11 16:29:16 PST 2019
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchattopadhyay/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D44A8A0-7015-A448-A5CC-F4C03BC3184A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5F8EDD-816A-6349-9B67-A47628089730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{26E92A9D-7BD1-914F-959E-FC63F09E2183}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$47</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="117">
   <si>
     <t>website</t>
   </si>
@@ -379,6 +379,12 @@
   </si>
   <si>
     <t>https://github.com/likarajo/text2number</t>
+  </si>
+  <si>
+    <t>movie_sentiment</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/movie_sentiment</t>
   </si>
 </sst>
 </file>
@@ -749,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2CE227-055B-2D42-8D36-FD50B0BC9862}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -873,7 +879,7 @@
         <v>95</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -881,10 +887,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>201</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
         <v>91</v>
@@ -893,10 +899,7 @@
         <v>95</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -904,10 +907,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>91</v>
@@ -916,21 +919,21 @@
         <v>95</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
-        <v>203</v>
+      <c r="B8">
+        <v>202</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>91</v>
@@ -939,30 +942,33 @@
         <v>95</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>301</v>
+      <c r="B9" s="3">
+        <v>203</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
         <v>95</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -970,10 +976,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>92</v>
@@ -982,18 +988,18 @@
         <v>95</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>401</v>
+      <c r="B11">
+        <v>302</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>92</v>
@@ -1002,7 +1008,7 @@
         <v>95</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1010,30 +1016,30 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E12" t="s">
         <v>95</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>501</v>
+      <c r="B13" s="3">
+        <v>402</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="D13" t="s">
         <v>91</v>
@@ -1042,41 +1048,41 @@
         <v>95</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
-        <v>502</v>
+      <c r="B14">
+        <v>501</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
         <v>95</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>503</v>
+      <c r="B15" s="3">
+        <v>502</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
         <v>92</v>
@@ -1085,7 +1091,7 @@
         <v>95</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1093,10 +1099,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
         <v>92</v>
@@ -1105,18 +1111,18 @@
         <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
-        <v>505</v>
+      <c r="B17">
+        <v>504</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
         <v>92</v>
@@ -1125,18 +1131,18 @@
         <v>95</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>506</v>
+      <c r="B18" s="3">
+        <v>505</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
         <v>92</v>
@@ -1145,7 +1151,7 @@
         <v>95</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1153,19 +1159,19 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E19" t="s">
         <v>95</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1173,10 +1179,10 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
         <v>91</v>
@@ -1185,7 +1191,7 @@
         <v>95</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1193,19 +1199,19 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" t="s">
         <v>95</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1213,10 +1219,10 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>601</v>
+        <v>509</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
         <v>92</v>
@@ -1225,7 +1231,7 @@
         <v>95</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1233,10 +1239,10 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
         <v>92</v>
@@ -1245,7 +1251,7 @@
         <v>95</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1253,10 +1259,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
         <v>92</v>
@@ -1265,7 +1271,7 @@
         <v>95</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1273,10 +1279,10 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
         <v>92</v>
@@ -1285,27 +1291,27 @@
         <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
-        <v>605</v>
+      <c r="B26">
+        <v>604</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
         <v>95</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1313,10 +1319,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="3">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
         <v>91</v>
@@ -1325,10 +1331,7 @@
         <v>95</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1336,10 +1339,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="3">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
         <v>91</v>
@@ -1348,10 +1351,10 @@
         <v>95</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1359,10 +1362,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="3">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
         <v>91</v>
@@ -1371,7 +1374,10 @@
         <v>95</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1379,19 +1385,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="3">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E30" t="s">
         <v>95</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1399,10 +1405,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="3">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
         <v>92</v>
@@ -1411,41 +1417,38 @@
         <v>95</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32">
-        <v>701</v>
+      <c r="B32" s="3">
+        <v>610</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E32" t="s">
         <v>95</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="3">
-        <v>702</v>
+      <c r="B33">
+        <v>701</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
         <v>91</v>
@@ -1454,27 +1457,30 @@
         <v>95</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>703</v>
+      <c r="B34" s="3">
+        <v>702</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E34" t="s">
         <v>95</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1482,10 +1488,10 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D35" t="s">
         <v>93</v>
@@ -1494,7 +1500,7 @@
         <v>95</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1502,19 +1508,19 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E36" t="s">
-        <v>103</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1522,10 +1528,10 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D37" t="s">
         <v>91</v>
@@ -1534,7 +1540,7 @@
         <v>103</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1542,22 +1548,19 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>801</v>
+        <v>706</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
         <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>95</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1565,31 +1568,33 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
         <v>91</v>
       </c>
       <c r="E39" t="s">
-        <v>103</v>
-      </c>
-      <c r="F39" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G39" s="1" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="3">
-        <v>803</v>
+      <c r="B40">
+        <v>802</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D40" t="s">
         <v>91</v>
@@ -1597,28 +1602,29 @@
       <c r="E40" t="s">
         <v>103</v>
       </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41">
-        <v>804</v>
+      <c r="B41" s="3">
+        <v>803</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E41" t="s">
         <v>103</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1629,16 +1635,16 @@
         <v>804</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E42" t="s">
         <v>103</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1646,19 +1652,19 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E43" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>72</v>
+        <v>103</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1666,19 +1672,19 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>901</v>
+        <v>805</v>
       </c>
       <c r="C44" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="D44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E44" t="s">
-        <v>103</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1686,22 +1692,19 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C45" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D45" t="s">
         <v>91</v>
       </c>
       <c r="E45" t="s">
-        <v>95</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1709,91 +1712,115 @@
         <v>45</v>
       </c>
       <c r="B46">
+        <v>902</v>
+      </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" t="s">
+        <v>95</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
         <v>903</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>34</v>
       </c>
-      <c r="D46" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" s="1" t="s">
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" t="s">
+        <v>95</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G46" xr:uid="{27AC6761-2437-C441-907E-B1FB733C8BAA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G46">
+  <autoFilter ref="B1:G47" xr:uid="{27AC6761-2437-C441-907E-B1FB733C8BAA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G47">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G46">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G47">
     <sortCondition ref="B1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" xr:uid="{E26AB3C4-29AE-204B-97A1-8F7175E3530D}"/>
-    <hyperlink ref="F13" r:id="rId2" xr:uid="{20C7D150-9462-1F41-AAB7-2A899F9C969A}"/>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{E26AB3C4-29AE-204B-97A1-8F7175E3530D}"/>
+    <hyperlink ref="F14" r:id="rId2" xr:uid="{20C7D150-9462-1F41-AAB7-2A899F9C969A}"/>
     <hyperlink ref="F5" r:id="rId3" xr:uid="{62DFB431-E49A-4741-B60E-DA27CFC68C72}"/>
-    <hyperlink ref="F14" r:id="rId4" xr:uid="{8506591B-A62F-6948-8F5E-FAB4DE06D345}"/>
-    <hyperlink ref="F19" r:id="rId5" xr:uid="{7B4333D3-C25D-3144-87C0-B86DA456F7A0}"/>
-    <hyperlink ref="F20" r:id="rId6" xr:uid="{6F8B3503-4C3A-DC40-8109-C9D396669308}"/>
-    <hyperlink ref="F6" r:id="rId7" xr:uid="{E11F3A2B-4236-C240-B3A5-B3577F908F63}"/>
-    <hyperlink ref="F22" r:id="rId8" xr:uid="{208F8125-58C4-4848-9C44-457B5CA9C713}"/>
-    <hyperlink ref="F27" r:id="rId9" xr:uid="{3F4F2A3A-2C07-1A42-AC3D-471388B48825}"/>
-    <hyperlink ref="F28" r:id="rId10" xr:uid="{119BF651-F8C7-C24B-BA6B-34B978975A37}"/>
-    <hyperlink ref="F32" r:id="rId11" xr:uid="{2CCAB83E-F41F-B24B-90B4-A0DB21E63EAC}"/>
-    <hyperlink ref="F38" r:id="rId12" xr:uid="{0826D0C0-8E81-C044-9D15-BC27CA346E4D}"/>
-    <hyperlink ref="F31" r:id="rId13" xr:uid="{4DDE0179-60BD-8D4F-9D6C-2A707E2A6ABF}"/>
-    <hyperlink ref="F7" r:id="rId14" xr:uid="{0317F90B-9CF5-D440-98C2-9DD3D8CD4360}"/>
-    <hyperlink ref="F25" r:id="rId15" xr:uid="{B0FDC84E-194C-CA4A-B974-8821AB0DA033}"/>
-    <hyperlink ref="F18" r:id="rId16" xr:uid="{5C69EB99-4BB2-6C40-B120-40DC6CEA8E3D}"/>
+    <hyperlink ref="F15" r:id="rId4" xr:uid="{8506591B-A62F-6948-8F5E-FAB4DE06D345}"/>
+    <hyperlink ref="F20" r:id="rId5" xr:uid="{7B4333D3-C25D-3144-87C0-B86DA456F7A0}"/>
+    <hyperlink ref="F21" r:id="rId6" xr:uid="{6F8B3503-4C3A-DC40-8109-C9D396669308}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{E11F3A2B-4236-C240-B3A5-B3577F908F63}"/>
+    <hyperlink ref="F23" r:id="rId8" xr:uid="{208F8125-58C4-4848-9C44-457B5CA9C713}"/>
+    <hyperlink ref="F28" r:id="rId9" xr:uid="{3F4F2A3A-2C07-1A42-AC3D-471388B48825}"/>
+    <hyperlink ref="F29" r:id="rId10" xr:uid="{119BF651-F8C7-C24B-BA6B-34B978975A37}"/>
+    <hyperlink ref="F33" r:id="rId11" xr:uid="{2CCAB83E-F41F-B24B-90B4-A0DB21E63EAC}"/>
+    <hyperlink ref="F39" r:id="rId12" xr:uid="{0826D0C0-8E81-C044-9D15-BC27CA346E4D}"/>
+    <hyperlink ref="F32" r:id="rId13" xr:uid="{4DDE0179-60BD-8D4F-9D6C-2A707E2A6ABF}"/>
+    <hyperlink ref="F8" r:id="rId14" xr:uid="{0317F90B-9CF5-D440-98C2-9DD3D8CD4360}"/>
+    <hyperlink ref="F26" r:id="rId15" xr:uid="{B0FDC84E-194C-CA4A-B974-8821AB0DA033}"/>
+    <hyperlink ref="F19" r:id="rId16" xr:uid="{5C69EB99-4BB2-6C40-B120-40DC6CEA8E3D}"/>
     <hyperlink ref="F2" r:id="rId17" xr:uid="{F9CDDCEB-59CD-AE47-A149-9CC74B550FEC}"/>
     <hyperlink ref="F3" r:id="rId18" xr:uid="{DE3B3CAA-EE98-3047-8B1C-3EEDFEAD7F28}"/>
     <hyperlink ref="F4" r:id="rId19" xr:uid="{3C4A7730-5B0F-F648-B13F-492DD0C989D9}"/>
-    <hyperlink ref="F17" r:id="rId20" xr:uid="{C1E695B0-BCA2-C543-ACE5-568C9F0303B1}"/>
-    <hyperlink ref="F29" r:id="rId21" xr:uid="{69EB5850-A79D-2249-8859-15359590B6A7}"/>
-    <hyperlink ref="F24" r:id="rId22" xr:uid="{C61A74F0-4B76-0C4E-BB52-AC63D005FD62}"/>
-    <hyperlink ref="F23" r:id="rId23" xr:uid="{81A92251-C09C-E44E-9A36-C9FE15E5FCD8}"/>
-    <hyperlink ref="F30" r:id="rId24" xr:uid="{F4F55930-9ED7-EA4F-BCBD-BCFEE7610B82}"/>
-    <hyperlink ref="F21" r:id="rId25" xr:uid="{0091B4FD-E7C4-1B4D-9203-8698BC24D565}"/>
-    <hyperlink ref="F33" r:id="rId26" xr:uid="{EB6B87D1-21E1-FC4E-B405-2E1E5231BF06}"/>
-    <hyperlink ref="F11" r:id="rId27" xr:uid="{71F90D41-9C86-E340-936E-3BB9C8F90010}"/>
-    <hyperlink ref="F15" r:id="rId28" xr:uid="{3DB60B42-7507-6C4E-BDAE-4CFDF2EB9C4B}"/>
-    <hyperlink ref="F26" r:id="rId29" xr:uid="{DE0DD6CB-D570-6945-B428-B9331B5F7EBD}"/>
-    <hyperlink ref="F16" r:id="rId30" xr:uid="{FEFB8575-764E-9449-AA25-D9D9E8089739}"/>
-    <hyperlink ref="F9" r:id="rId31" xr:uid="{D26F3756-D827-C34C-94BF-A5B4EB60366B}"/>
-    <hyperlink ref="F10" r:id="rId32" xr:uid="{784A9FC5-FAB0-B844-BE6A-3AF588A130C9}"/>
-    <hyperlink ref="F43" r:id="rId33" xr:uid="{EB6D586F-57BF-DD4A-8A35-36111ACF2E34}"/>
-    <hyperlink ref="F45" r:id="rId34" xr:uid="{4FE78F82-E051-BD41-AF8D-290EBCE2FD87}"/>
-    <hyperlink ref="F46" r:id="rId35" xr:uid="{EFC9C5A7-AB7E-6445-B238-3F6B90ECD054}"/>
-    <hyperlink ref="F34" r:id="rId36" xr:uid="{63617CDE-2E2D-AD4B-A08D-0848E898DD47}"/>
-    <hyperlink ref="F35" r:id="rId37" xr:uid="{3F4D27CA-6390-D84B-B25B-184101CE06FA}"/>
-    <hyperlink ref="G8" r:id="rId38" xr:uid="{07E7E11C-8841-7748-BFFF-540D5BB62B39}"/>
-    <hyperlink ref="G13" r:id="rId39" xr:uid="{41C80DDC-B435-E44A-B9FF-4AF4DE2F5656}"/>
-    <hyperlink ref="G6" r:id="rId40" xr:uid="{9F0DCD01-87D0-6A40-AE3F-32FC101B7188}"/>
-    <hyperlink ref="G27" r:id="rId41" xr:uid="{197BB746-FF15-2148-98BE-5BB0F1F85567}"/>
-    <hyperlink ref="G28" r:id="rId42" xr:uid="{C77A6773-BBA6-584C-8DAC-DE08233409B2}"/>
-    <hyperlink ref="G32" r:id="rId43" xr:uid="{7FC8D046-4E44-AD48-B3AC-C616091F1C3A}"/>
-    <hyperlink ref="G38" r:id="rId44" xr:uid="{F25E562D-AAF9-4041-B937-A59BAFE18EC5}"/>
-    <hyperlink ref="G7" r:id="rId45" xr:uid="{B3DC7E65-8B74-914F-93A8-6005B22982A3}"/>
+    <hyperlink ref="F18" r:id="rId20" xr:uid="{C1E695B0-BCA2-C543-ACE5-568C9F0303B1}"/>
+    <hyperlink ref="F30" r:id="rId21" xr:uid="{69EB5850-A79D-2249-8859-15359590B6A7}"/>
+    <hyperlink ref="F25" r:id="rId22" xr:uid="{C61A74F0-4B76-0C4E-BB52-AC63D005FD62}"/>
+    <hyperlink ref="F24" r:id="rId23" xr:uid="{81A92251-C09C-E44E-9A36-C9FE15E5FCD8}"/>
+    <hyperlink ref="F31" r:id="rId24" xr:uid="{F4F55930-9ED7-EA4F-BCBD-BCFEE7610B82}"/>
+    <hyperlink ref="F22" r:id="rId25" xr:uid="{0091B4FD-E7C4-1B4D-9203-8698BC24D565}"/>
+    <hyperlink ref="F34" r:id="rId26" xr:uid="{EB6B87D1-21E1-FC4E-B405-2E1E5231BF06}"/>
+    <hyperlink ref="F12" r:id="rId27" xr:uid="{71F90D41-9C86-E340-936E-3BB9C8F90010}"/>
+    <hyperlink ref="F16" r:id="rId28" xr:uid="{3DB60B42-7507-6C4E-BDAE-4CFDF2EB9C4B}"/>
+    <hyperlink ref="F27" r:id="rId29" xr:uid="{DE0DD6CB-D570-6945-B428-B9331B5F7EBD}"/>
+    <hyperlink ref="F17" r:id="rId30" xr:uid="{FEFB8575-764E-9449-AA25-D9D9E8089739}"/>
+    <hyperlink ref="F10" r:id="rId31" xr:uid="{D26F3756-D827-C34C-94BF-A5B4EB60366B}"/>
+    <hyperlink ref="F11" r:id="rId32" xr:uid="{784A9FC5-FAB0-B844-BE6A-3AF588A130C9}"/>
+    <hyperlink ref="F44" r:id="rId33" xr:uid="{EB6D586F-57BF-DD4A-8A35-36111ACF2E34}"/>
+    <hyperlink ref="F46" r:id="rId34" xr:uid="{4FE78F82-E051-BD41-AF8D-290EBCE2FD87}"/>
+    <hyperlink ref="F47" r:id="rId35" xr:uid="{EFC9C5A7-AB7E-6445-B238-3F6B90ECD054}"/>
+    <hyperlink ref="F35" r:id="rId36" xr:uid="{63617CDE-2E2D-AD4B-A08D-0848E898DD47}"/>
+    <hyperlink ref="F36" r:id="rId37" xr:uid="{3F4D27CA-6390-D84B-B25B-184101CE06FA}"/>
+    <hyperlink ref="G9" r:id="rId38" xr:uid="{07E7E11C-8841-7748-BFFF-540D5BB62B39}"/>
+    <hyperlink ref="G14" r:id="rId39" xr:uid="{41C80DDC-B435-E44A-B9FF-4AF4DE2F5656}"/>
+    <hyperlink ref="G7" r:id="rId40" xr:uid="{9F0DCD01-87D0-6A40-AE3F-32FC101B7188}"/>
+    <hyperlink ref="G28" r:id="rId41" xr:uid="{197BB746-FF15-2148-98BE-5BB0F1F85567}"/>
+    <hyperlink ref="G29" r:id="rId42" xr:uid="{C77A6773-BBA6-584C-8DAC-DE08233409B2}"/>
+    <hyperlink ref="G33" r:id="rId43" xr:uid="{7FC8D046-4E44-AD48-B3AC-C616091F1C3A}"/>
+    <hyperlink ref="G39" r:id="rId44" xr:uid="{F25E562D-AAF9-4041-B937-A59BAFE18EC5}"/>
+    <hyperlink ref="G8" r:id="rId45" xr:uid="{B3DC7E65-8B74-914F-93A8-6005B22982A3}"/>
     <hyperlink ref="G2" r:id="rId46" xr:uid="{843CA431-F6E9-1B4D-845E-601D7EDB0BB1}"/>
     <hyperlink ref="G3" r:id="rId47" xr:uid="{4D5CA3E4-8FD4-DE4A-83B2-0E8DDA142970}"/>
     <hyperlink ref="G4" r:id="rId48" xr:uid="{F45701A4-E062-F544-AEFE-3543E8569B6E}"/>
-    <hyperlink ref="G45" r:id="rId49" xr:uid="{985334CD-1972-8442-AD5A-14F3D57E92CF}"/>
-    <hyperlink ref="G46" r:id="rId50" xr:uid="{5556EC84-5DAB-B246-9C73-76642D572382}"/>
-    <hyperlink ref="G44" r:id="rId51" xr:uid="{51C1EF83-209F-024C-B3DA-10B36D1E5A4C}"/>
-    <hyperlink ref="G37" r:id="rId52" xr:uid="{BED6B18A-333C-D348-9DA2-FBE4265E3C32}"/>
-    <hyperlink ref="G36" r:id="rId53" xr:uid="{68C79AD3-9ED9-684B-BA88-B3D3EE552B52}"/>
-    <hyperlink ref="G42" r:id="rId54" xr:uid="{149FC972-472B-6F48-BC30-B43708381DDC}"/>
-    <hyperlink ref="G41" r:id="rId55" xr:uid="{6E323EF5-0E5A-5B4C-BD17-16A6D0E2C053}"/>
-    <hyperlink ref="G40" r:id="rId56" xr:uid="{96FE3BD0-D39E-7A4F-953E-7831D516D31B}"/>
-    <hyperlink ref="F12" r:id="rId57" xr:uid="{D6022A27-41D7-5246-8EF9-8E2A4D9AC1A6}"/>
+    <hyperlink ref="G46" r:id="rId49" xr:uid="{985334CD-1972-8442-AD5A-14F3D57E92CF}"/>
+    <hyperlink ref="G47" r:id="rId50" xr:uid="{5556EC84-5DAB-B246-9C73-76642D572382}"/>
+    <hyperlink ref="G45" r:id="rId51" xr:uid="{51C1EF83-209F-024C-B3DA-10B36D1E5A4C}"/>
+    <hyperlink ref="G38" r:id="rId52" xr:uid="{BED6B18A-333C-D348-9DA2-FBE4265E3C32}"/>
+    <hyperlink ref="G37" r:id="rId53" xr:uid="{68C79AD3-9ED9-684B-BA88-B3D3EE552B52}"/>
+    <hyperlink ref="G43" r:id="rId54" xr:uid="{149FC972-472B-6F48-BC30-B43708381DDC}"/>
+    <hyperlink ref="G42" r:id="rId55" xr:uid="{6E323EF5-0E5A-5B4C-BD17-16A6D0E2C053}"/>
+    <hyperlink ref="G41" r:id="rId56" xr:uid="{96FE3BD0-D39E-7A4F-953E-7831D516D31B}"/>
+    <hyperlink ref="F13" r:id="rId57" xr:uid="{D6022A27-41D7-5246-8EF9-8E2A4D9AC1A6}"/>
+    <hyperlink ref="F6" r:id="rId58" xr:uid="{6C9B7A1E-278F-074C-9373-5B8E9C5D9D34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Site rebuild Mon Dec 30 12:02:49 IST 2019
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchattopadhyay/Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/likarajo/#GITHUB/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5F8EDD-816A-6349-9B67-A47628089730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18260DFB-E7F9-1D49-BDA0-D53E06915FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{26E92A9D-7BD1-914F-959E-FC63F09E2183}"/>
+    <workbookView xWindow="2940" yWindow="460" windowWidth="25480" windowHeight="16620" xr2:uid="{26E92A9D-7BD1-914F-959E-FC63F09E2183}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$55</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="133">
   <si>
     <t>website</t>
   </si>
@@ -385,6 +385,54 @@
   </si>
   <si>
     <t>https://github.com/likarajo/movie_sentiment</t>
+  </si>
+  <si>
+    <t>petrol_consumption</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/petrol_consumption</t>
+  </si>
+  <si>
+    <t>car_evaluation</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/car_evaluation</t>
+  </si>
+  <si>
+    <t>passengers_count</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/passengers_count</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/customer_churn</t>
+  </si>
+  <si>
+    <t>customer_churn</t>
+  </si>
+  <si>
+    <t>language_translation</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/language_translation</t>
+  </si>
+  <si>
+    <t>text_generation</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/text_generation</t>
+  </si>
+  <si>
+    <t>comment_toxicity</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/comment_toxicity</t>
+  </si>
+  <si>
+    <t>business_reviews</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/business_reviews</t>
   </si>
 </sst>
 </file>
@@ -755,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2CE227-055B-2D42-8D36-FD50B0BC9862}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,7 +927,7 @@
         <v>95</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -899,7 +947,7 @@
         <v>95</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -907,10 +955,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>201</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
         <v>91</v>
@@ -919,10 +967,7 @@
         <v>95</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -930,10 +975,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>202</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="D8" t="s">
         <v>91</v>
@@ -942,21 +987,18 @@
         <v>95</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <v>203</v>
+      <c r="B9">
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
         <v>91</v>
@@ -965,10 +1007,7 @@
         <v>95</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -976,19 +1015,19 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>301</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" t="s">
         <v>95</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -996,50 +1035,50 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>302</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
         <v>95</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
-        <v>401</v>
+      <c r="B12">
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
         <v>95</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <v>402</v>
+      <c r="B13">
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
         <v>91</v>
@@ -1048,7 +1087,7 @@
         <v>95</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1056,10 +1095,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>501</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="D14" t="s">
         <v>91</v>
@@ -1068,30 +1107,30 @@
         <v>95</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
-        <v>502</v>
+      <c r="B15">
+        <v>201</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
         <v>95</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1099,50 +1138,56 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>503</v>
+        <v>202</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
         <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>504</v>
+      <c r="B17" s="3">
+        <v>203</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
         <v>95</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>69</v>
+        <v>40</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
-        <v>505</v>
+      <c r="B18">
+        <v>301</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
         <v>92</v>
@@ -1151,7 +1196,7 @@
         <v>95</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1159,10 +1204,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>506</v>
+        <v>302</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
         <v>92</v>
@@ -1171,38 +1216,38 @@
         <v>95</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>507</v>
+      <c r="B20" s="3">
+        <v>401</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E20" t="s">
         <v>95</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>508</v>
+      <c r="B21" s="3">
+        <v>402</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="D21" t="s">
         <v>91</v>
@@ -1211,7 +1256,7 @@
         <v>95</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1219,30 +1264,33 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
         <v>95</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>601</v>
+      <c r="B23" s="3">
+        <v>502</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
         <v>92</v>
@@ -1251,7 +1299,7 @@
         <v>95</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1259,10 +1307,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>602</v>
+        <v>503</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
         <v>92</v>
@@ -1271,7 +1319,7 @@
         <v>95</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1279,10 +1327,10 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>603</v>
+        <v>504</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
         <v>92</v>
@@ -1291,18 +1339,18 @@
         <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>604</v>
+      <c r="B26" s="3">
+        <v>505</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
         <v>92</v>
@@ -1311,38 +1359,38 @@
         <v>95</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
-        <v>605</v>
+      <c r="B27">
+        <v>506</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
         <v>95</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
-        <v>606</v>
+      <c r="B28">
+        <v>507</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
         <v>91</v>
@@ -1351,21 +1399,18 @@
         <v>95</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
-        <v>607</v>
+      <c r="B29">
+        <v>508</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
         <v>91</v>
@@ -1374,41 +1419,38 @@
         <v>95</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
-        <v>608</v>
+      <c r="B30">
+        <v>509</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E30" t="s">
         <v>95</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
-        <v>609</v>
+      <c r="B31">
+        <v>601</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
         <v>92</v>
@@ -1417,18 +1459,18 @@
         <v>95</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
-        <v>610</v>
+      <c r="B32">
+        <v>602</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D32" t="s">
         <v>92</v>
@@ -1437,7 +1479,7 @@
         <v>95</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1445,206 +1487,208 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>701</v>
+        <v>603</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
         <v>95</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="3">
-        <v>702</v>
+      <c r="B34">
+        <v>604</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E34" t="s">
         <v>95</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35">
-        <v>703</v>
+      <c r="B35" s="3">
+        <v>605</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E35" t="s">
         <v>95</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36">
-        <v>704</v>
+      <c r="B36" s="3">
+        <v>606</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E36" t="s">
         <v>95</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>76</v>
+        <v>48</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37">
-        <v>705</v>
+      <c r="B37" s="3">
+        <v>607</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="D37" t="s">
         <v>91</v>
       </c>
       <c r="E37" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38">
-        <v>706</v>
+      <c r="B38" s="3">
+        <v>608</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="D38" t="s">
         <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>103</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39">
-        <v>801</v>
+      <c r="B39" s="3">
+        <v>609</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E39" t="s">
         <v>95</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40">
-        <v>802</v>
+      <c r="B40" s="3">
+        <v>610</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E40" t="s">
-        <v>103</v>
-      </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="3">
-        <v>803</v>
+      <c r="B41">
+        <v>701</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
         <v>91</v>
       </c>
       <c r="E41" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42">
-        <v>804</v>
+      <c r="B42" s="3">
+        <v>702</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="D42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E42" t="s">
-        <v>103</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1652,19 +1696,19 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>804</v>
+        <v>703</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="D43" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E43" t="s">
-        <v>103</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1672,19 +1716,19 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>805</v>
+        <v>704</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D44" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E44" t="s">
         <v>95</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1692,10 +1736,10 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>901</v>
+        <v>705</v>
       </c>
       <c r="C45" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D45" t="s">
         <v>91</v>
@@ -1704,7 +1748,7 @@
         <v>103</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1712,22 +1756,19 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>902</v>
+        <v>706</v>
       </c>
       <c r="C46" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="D46" t="s">
         <v>91</v>
       </c>
       <c r="E46" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1735,92 +1776,267 @@
         <v>46</v>
       </c>
       <c r="B47">
+        <v>801</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" t="s">
+        <v>95</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>802</v>
+      </c>
+      <c r="C48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" t="s">
+        <v>103</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3">
+        <v>803</v>
+      </c>
+      <c r="C49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" t="s">
+        <v>103</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>804</v>
+      </c>
+      <c r="C50" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50" t="s">
+        <v>103</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>804</v>
+      </c>
+      <c r="C51" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" t="s">
+        <v>103</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>805</v>
+      </c>
+      <c r="C52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" t="s">
+        <v>95</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>901</v>
+      </c>
+      <c r="C53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E53" t="s">
+        <v>103</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>902</v>
+      </c>
+      <c r="C54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" t="s">
+        <v>95</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
         <v>903</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C55" t="s">
         <v>34</v>
       </c>
-      <c r="D47" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" t="s">
-        <v>95</v>
-      </c>
-      <c r="F47" s="1" t="s">
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" t="s">
+        <v>95</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G47" xr:uid="{27AC6761-2437-C441-907E-B1FB733C8BAA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G47">
+  <autoFilter ref="B1:G55" xr:uid="{27AC6761-2437-C441-907E-B1FB733C8BAA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G55">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G47">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G55">
     <sortCondition ref="B1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F9" r:id="rId1" xr:uid="{E26AB3C4-29AE-204B-97A1-8F7175E3530D}"/>
-    <hyperlink ref="F14" r:id="rId2" xr:uid="{20C7D150-9462-1F41-AAB7-2A899F9C969A}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{62DFB431-E49A-4741-B60E-DA27CFC68C72}"/>
-    <hyperlink ref="F15" r:id="rId4" xr:uid="{8506591B-A62F-6948-8F5E-FAB4DE06D345}"/>
-    <hyperlink ref="F20" r:id="rId5" xr:uid="{7B4333D3-C25D-3144-87C0-B86DA456F7A0}"/>
-    <hyperlink ref="F21" r:id="rId6" xr:uid="{6F8B3503-4C3A-DC40-8109-C9D396669308}"/>
-    <hyperlink ref="F7" r:id="rId7" xr:uid="{E11F3A2B-4236-C240-B3A5-B3577F908F63}"/>
-    <hyperlink ref="F23" r:id="rId8" xr:uid="{208F8125-58C4-4848-9C44-457B5CA9C713}"/>
-    <hyperlink ref="F28" r:id="rId9" xr:uid="{3F4F2A3A-2C07-1A42-AC3D-471388B48825}"/>
-    <hyperlink ref="F29" r:id="rId10" xr:uid="{119BF651-F8C7-C24B-BA6B-34B978975A37}"/>
-    <hyperlink ref="F33" r:id="rId11" xr:uid="{2CCAB83E-F41F-B24B-90B4-A0DB21E63EAC}"/>
-    <hyperlink ref="F39" r:id="rId12" xr:uid="{0826D0C0-8E81-C044-9D15-BC27CA346E4D}"/>
-    <hyperlink ref="F32" r:id="rId13" xr:uid="{4DDE0179-60BD-8D4F-9D6C-2A707E2A6ABF}"/>
-    <hyperlink ref="F8" r:id="rId14" xr:uid="{0317F90B-9CF5-D440-98C2-9DD3D8CD4360}"/>
-    <hyperlink ref="F26" r:id="rId15" xr:uid="{B0FDC84E-194C-CA4A-B974-8821AB0DA033}"/>
-    <hyperlink ref="F19" r:id="rId16" xr:uid="{5C69EB99-4BB2-6C40-B120-40DC6CEA8E3D}"/>
+    <hyperlink ref="F17" r:id="rId1" xr:uid="{E26AB3C4-29AE-204B-97A1-8F7175E3530D}"/>
+    <hyperlink ref="F22" r:id="rId2" xr:uid="{20C7D150-9462-1F41-AAB7-2A899F9C969A}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{62DFB431-E49A-4741-B60E-DA27CFC68C72}"/>
+    <hyperlink ref="F23" r:id="rId4" xr:uid="{8506591B-A62F-6948-8F5E-FAB4DE06D345}"/>
+    <hyperlink ref="F28" r:id="rId5" xr:uid="{7B4333D3-C25D-3144-87C0-B86DA456F7A0}"/>
+    <hyperlink ref="F29" r:id="rId6" xr:uid="{6F8B3503-4C3A-DC40-8109-C9D396669308}"/>
+    <hyperlink ref="F15" r:id="rId7" xr:uid="{E11F3A2B-4236-C240-B3A5-B3577F908F63}"/>
+    <hyperlink ref="F31" r:id="rId8" xr:uid="{208F8125-58C4-4848-9C44-457B5CA9C713}"/>
+    <hyperlink ref="F36" r:id="rId9" xr:uid="{3F4F2A3A-2C07-1A42-AC3D-471388B48825}"/>
+    <hyperlink ref="F37" r:id="rId10" xr:uid="{119BF651-F8C7-C24B-BA6B-34B978975A37}"/>
+    <hyperlink ref="F41" r:id="rId11" xr:uid="{2CCAB83E-F41F-B24B-90B4-A0DB21E63EAC}"/>
+    <hyperlink ref="F47" r:id="rId12" xr:uid="{0826D0C0-8E81-C044-9D15-BC27CA346E4D}"/>
+    <hyperlink ref="F40" r:id="rId13" xr:uid="{4DDE0179-60BD-8D4F-9D6C-2A707E2A6ABF}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{0317F90B-9CF5-D440-98C2-9DD3D8CD4360}"/>
+    <hyperlink ref="F34" r:id="rId15" xr:uid="{B0FDC84E-194C-CA4A-B974-8821AB0DA033}"/>
+    <hyperlink ref="F27" r:id="rId16" xr:uid="{5C69EB99-4BB2-6C40-B120-40DC6CEA8E3D}"/>
     <hyperlink ref="F2" r:id="rId17" xr:uid="{F9CDDCEB-59CD-AE47-A149-9CC74B550FEC}"/>
     <hyperlink ref="F3" r:id="rId18" xr:uid="{DE3B3CAA-EE98-3047-8B1C-3EEDFEAD7F28}"/>
     <hyperlink ref="F4" r:id="rId19" xr:uid="{3C4A7730-5B0F-F648-B13F-492DD0C989D9}"/>
-    <hyperlink ref="F18" r:id="rId20" xr:uid="{C1E695B0-BCA2-C543-ACE5-568C9F0303B1}"/>
-    <hyperlink ref="F30" r:id="rId21" xr:uid="{69EB5850-A79D-2249-8859-15359590B6A7}"/>
-    <hyperlink ref="F25" r:id="rId22" xr:uid="{C61A74F0-4B76-0C4E-BB52-AC63D005FD62}"/>
-    <hyperlink ref="F24" r:id="rId23" xr:uid="{81A92251-C09C-E44E-9A36-C9FE15E5FCD8}"/>
-    <hyperlink ref="F31" r:id="rId24" xr:uid="{F4F55930-9ED7-EA4F-BCBD-BCFEE7610B82}"/>
-    <hyperlink ref="F22" r:id="rId25" xr:uid="{0091B4FD-E7C4-1B4D-9203-8698BC24D565}"/>
-    <hyperlink ref="F34" r:id="rId26" xr:uid="{EB6B87D1-21E1-FC4E-B405-2E1E5231BF06}"/>
-    <hyperlink ref="F12" r:id="rId27" xr:uid="{71F90D41-9C86-E340-936E-3BB9C8F90010}"/>
-    <hyperlink ref="F16" r:id="rId28" xr:uid="{3DB60B42-7507-6C4E-BDAE-4CFDF2EB9C4B}"/>
-    <hyperlink ref="F27" r:id="rId29" xr:uid="{DE0DD6CB-D570-6945-B428-B9331B5F7EBD}"/>
-    <hyperlink ref="F17" r:id="rId30" xr:uid="{FEFB8575-764E-9449-AA25-D9D9E8089739}"/>
-    <hyperlink ref="F10" r:id="rId31" xr:uid="{D26F3756-D827-C34C-94BF-A5B4EB60366B}"/>
-    <hyperlink ref="F11" r:id="rId32" xr:uid="{784A9FC5-FAB0-B844-BE6A-3AF588A130C9}"/>
-    <hyperlink ref="F44" r:id="rId33" xr:uid="{EB6D586F-57BF-DD4A-8A35-36111ACF2E34}"/>
-    <hyperlink ref="F46" r:id="rId34" xr:uid="{4FE78F82-E051-BD41-AF8D-290EBCE2FD87}"/>
-    <hyperlink ref="F47" r:id="rId35" xr:uid="{EFC9C5A7-AB7E-6445-B238-3F6B90ECD054}"/>
-    <hyperlink ref="F35" r:id="rId36" xr:uid="{63617CDE-2E2D-AD4B-A08D-0848E898DD47}"/>
-    <hyperlink ref="F36" r:id="rId37" xr:uid="{3F4D27CA-6390-D84B-B25B-184101CE06FA}"/>
-    <hyperlink ref="G9" r:id="rId38" xr:uid="{07E7E11C-8841-7748-BFFF-540D5BB62B39}"/>
-    <hyperlink ref="G14" r:id="rId39" xr:uid="{41C80DDC-B435-E44A-B9FF-4AF4DE2F5656}"/>
-    <hyperlink ref="G7" r:id="rId40" xr:uid="{9F0DCD01-87D0-6A40-AE3F-32FC101B7188}"/>
-    <hyperlink ref="G28" r:id="rId41" xr:uid="{197BB746-FF15-2148-98BE-5BB0F1F85567}"/>
-    <hyperlink ref="G29" r:id="rId42" xr:uid="{C77A6773-BBA6-584C-8DAC-DE08233409B2}"/>
-    <hyperlink ref="G33" r:id="rId43" xr:uid="{7FC8D046-4E44-AD48-B3AC-C616091F1C3A}"/>
-    <hyperlink ref="G39" r:id="rId44" xr:uid="{F25E562D-AAF9-4041-B937-A59BAFE18EC5}"/>
-    <hyperlink ref="G8" r:id="rId45" xr:uid="{B3DC7E65-8B74-914F-93A8-6005B22982A3}"/>
+    <hyperlink ref="F26" r:id="rId20" xr:uid="{C1E695B0-BCA2-C543-ACE5-568C9F0303B1}"/>
+    <hyperlink ref="F38" r:id="rId21" xr:uid="{69EB5850-A79D-2249-8859-15359590B6A7}"/>
+    <hyperlink ref="F33" r:id="rId22" xr:uid="{C61A74F0-4B76-0C4E-BB52-AC63D005FD62}"/>
+    <hyperlink ref="F32" r:id="rId23" xr:uid="{81A92251-C09C-E44E-9A36-C9FE15E5FCD8}"/>
+    <hyperlink ref="F39" r:id="rId24" xr:uid="{F4F55930-9ED7-EA4F-BCBD-BCFEE7610B82}"/>
+    <hyperlink ref="F30" r:id="rId25" xr:uid="{0091B4FD-E7C4-1B4D-9203-8698BC24D565}"/>
+    <hyperlink ref="F42" r:id="rId26" xr:uid="{EB6B87D1-21E1-FC4E-B405-2E1E5231BF06}"/>
+    <hyperlink ref="F20" r:id="rId27" xr:uid="{71F90D41-9C86-E340-936E-3BB9C8F90010}"/>
+    <hyperlink ref="F24" r:id="rId28" xr:uid="{3DB60B42-7507-6C4E-BDAE-4CFDF2EB9C4B}"/>
+    <hyperlink ref="F35" r:id="rId29" xr:uid="{DE0DD6CB-D570-6945-B428-B9331B5F7EBD}"/>
+    <hyperlink ref="F25" r:id="rId30" xr:uid="{FEFB8575-764E-9449-AA25-D9D9E8089739}"/>
+    <hyperlink ref="F18" r:id="rId31" xr:uid="{D26F3756-D827-C34C-94BF-A5B4EB60366B}"/>
+    <hyperlink ref="F19" r:id="rId32" xr:uid="{784A9FC5-FAB0-B844-BE6A-3AF588A130C9}"/>
+    <hyperlink ref="F52" r:id="rId33" xr:uid="{EB6D586F-57BF-DD4A-8A35-36111ACF2E34}"/>
+    <hyperlink ref="F54" r:id="rId34" xr:uid="{4FE78F82-E051-BD41-AF8D-290EBCE2FD87}"/>
+    <hyperlink ref="F55" r:id="rId35" xr:uid="{EFC9C5A7-AB7E-6445-B238-3F6B90ECD054}"/>
+    <hyperlink ref="F43" r:id="rId36" xr:uid="{63617CDE-2E2D-AD4B-A08D-0848E898DD47}"/>
+    <hyperlink ref="F44" r:id="rId37" xr:uid="{3F4D27CA-6390-D84B-B25B-184101CE06FA}"/>
+    <hyperlink ref="G17" r:id="rId38" xr:uid="{07E7E11C-8841-7748-BFFF-540D5BB62B39}"/>
+    <hyperlink ref="G22" r:id="rId39" xr:uid="{41C80DDC-B435-E44A-B9FF-4AF4DE2F5656}"/>
+    <hyperlink ref="G15" r:id="rId40" xr:uid="{9F0DCD01-87D0-6A40-AE3F-32FC101B7188}"/>
+    <hyperlink ref="G36" r:id="rId41" xr:uid="{197BB746-FF15-2148-98BE-5BB0F1F85567}"/>
+    <hyperlink ref="G37" r:id="rId42" xr:uid="{C77A6773-BBA6-584C-8DAC-DE08233409B2}"/>
+    <hyperlink ref="G41" r:id="rId43" xr:uid="{7FC8D046-4E44-AD48-B3AC-C616091F1C3A}"/>
+    <hyperlink ref="G47" r:id="rId44" xr:uid="{F25E562D-AAF9-4041-B937-A59BAFE18EC5}"/>
+    <hyperlink ref="G16" r:id="rId45" xr:uid="{B3DC7E65-8B74-914F-93A8-6005B22982A3}"/>
     <hyperlink ref="G2" r:id="rId46" xr:uid="{843CA431-F6E9-1B4D-845E-601D7EDB0BB1}"/>
     <hyperlink ref="G3" r:id="rId47" xr:uid="{4D5CA3E4-8FD4-DE4A-83B2-0E8DDA142970}"/>
     <hyperlink ref="G4" r:id="rId48" xr:uid="{F45701A4-E062-F544-AEFE-3543E8569B6E}"/>
-    <hyperlink ref="G46" r:id="rId49" xr:uid="{985334CD-1972-8442-AD5A-14F3D57E92CF}"/>
-    <hyperlink ref="G47" r:id="rId50" xr:uid="{5556EC84-5DAB-B246-9C73-76642D572382}"/>
-    <hyperlink ref="G45" r:id="rId51" xr:uid="{51C1EF83-209F-024C-B3DA-10B36D1E5A4C}"/>
-    <hyperlink ref="G38" r:id="rId52" xr:uid="{BED6B18A-333C-D348-9DA2-FBE4265E3C32}"/>
-    <hyperlink ref="G37" r:id="rId53" xr:uid="{68C79AD3-9ED9-684B-BA88-B3D3EE552B52}"/>
-    <hyperlink ref="G43" r:id="rId54" xr:uid="{149FC972-472B-6F48-BC30-B43708381DDC}"/>
-    <hyperlink ref="G42" r:id="rId55" xr:uid="{6E323EF5-0E5A-5B4C-BD17-16A6D0E2C053}"/>
-    <hyperlink ref="G41" r:id="rId56" xr:uid="{96FE3BD0-D39E-7A4F-953E-7831D516D31B}"/>
-    <hyperlink ref="F13" r:id="rId57" xr:uid="{D6022A27-41D7-5246-8EF9-8E2A4D9AC1A6}"/>
-    <hyperlink ref="F6" r:id="rId58" xr:uid="{6C9B7A1E-278F-074C-9373-5B8E9C5D9D34}"/>
+    <hyperlink ref="G54" r:id="rId49" xr:uid="{985334CD-1972-8442-AD5A-14F3D57E92CF}"/>
+    <hyperlink ref="G55" r:id="rId50" xr:uid="{5556EC84-5DAB-B246-9C73-76642D572382}"/>
+    <hyperlink ref="G53" r:id="rId51" xr:uid="{51C1EF83-209F-024C-B3DA-10B36D1E5A4C}"/>
+    <hyperlink ref="G46" r:id="rId52" xr:uid="{BED6B18A-333C-D348-9DA2-FBE4265E3C32}"/>
+    <hyperlink ref="G45" r:id="rId53" xr:uid="{68C79AD3-9ED9-684B-BA88-B3D3EE552B52}"/>
+    <hyperlink ref="G51" r:id="rId54" xr:uid="{149FC972-472B-6F48-BC30-B43708381DDC}"/>
+    <hyperlink ref="G50" r:id="rId55" xr:uid="{6E323EF5-0E5A-5B4C-BD17-16A6D0E2C053}"/>
+    <hyperlink ref="G49" r:id="rId56" xr:uid="{96FE3BD0-D39E-7A4F-953E-7831D516D31B}"/>
+    <hyperlink ref="F21" r:id="rId57" xr:uid="{D6022A27-41D7-5246-8EF9-8E2A4D9AC1A6}"/>
+    <hyperlink ref="F5" r:id="rId58" xr:uid="{532705D3-72B5-C54F-B311-5B790A4C8170}"/>
+    <hyperlink ref="F10" r:id="rId59" xr:uid="{07F89B1F-6BF6-EC45-84D1-D16AABC8DE2F}"/>
+    <hyperlink ref="F9" r:id="rId60" xr:uid="{E2D8DF9F-F502-0243-964F-5B6E3821EB45}"/>
+    <hyperlink ref="F8" r:id="rId61" xr:uid="{CCBEA3C2-3A16-3748-91CF-54E21AA3849F}"/>
+    <hyperlink ref="F7" r:id="rId62" xr:uid="{0EB5657F-8B99-984F-9482-75C40E89916E}"/>
+    <hyperlink ref="F12" r:id="rId63" xr:uid="{19D732CA-E945-4443-BE0E-EEBC25D98642}"/>
+    <hyperlink ref="F11" r:id="rId64" xr:uid="{2D057E9E-BED0-6E4D-85F7-7DF9AF7C772D}"/>
+    <hyperlink ref="F13" r:id="rId65" xr:uid="{5338C8C7-0F3B-2447-83CB-A823FB7FA683}"/>
+    <hyperlink ref="F14" r:id="rId66" xr:uid="{C413640A-E27E-E24B-B726-4D512D306CE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Site rebuild Fri Jan 10 11:46:50 IST 2020
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/likarajo/#GITHUB/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18260DFB-E7F9-1D49-BDA0-D53E06915FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F51651A-0FEC-AE4B-8AD9-B487D633EDB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="460" windowWidth="25480" windowHeight="16620" xr2:uid="{26E92A9D-7BD1-914F-959E-FC63F09E2183}"/>
+    <workbookView xWindow="2540" yWindow="460" windowWidth="26260" windowHeight="16660" xr2:uid="{26E92A9D-7BD1-914F-959E-FC63F09E2183}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="151">
   <si>
     <t>website</t>
   </si>
@@ -433,6 +433,60 @@
   </si>
   <si>
     <t>https://github.com/likarajo/business_reviews</t>
+  </si>
+  <si>
+    <t>customer_targeting</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/customer_targeting</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/blackfriday_shopping</t>
+  </si>
+  <si>
+    <t>blackfriday_shopping</t>
+  </si>
+  <si>
+    <t>text_summarization</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/text_summarization</t>
+  </si>
+  <si>
+    <t>wine_quality</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/wine_quality</t>
+  </si>
+  <si>
+    <t>shopping_trends</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/shopping_trends</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/spam_sms</t>
+  </si>
+  <si>
+    <t>spam_sms</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/glass_type</t>
+  </si>
+  <si>
+    <t>glass_type</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/currencynote_authenticity</t>
+  </si>
+  <si>
+    <t>currencynote_authenticity</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/weather_prediction</t>
+  </si>
+  <si>
+    <t>weather_predcition</t>
   </si>
 </sst>
 </file>
@@ -803,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2CE227-055B-2D42-8D36-FD50B0BC9862}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1115,10 +1169,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>201</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>133</v>
       </c>
       <c r="D15" t="s">
         <v>91</v>
@@ -1127,10 +1181,7 @@
         <v>95</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1138,10 +1189,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>202</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
         <v>91</v>
@@ -1150,21 +1201,18 @@
         <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
-        <v>203</v>
+      <c r="B17">
+        <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="D17" t="s">
         <v>91</v>
@@ -1173,10 +1221,7 @@
         <v>95</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>77</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1184,19 +1229,19 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>301</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E18" t="s">
         <v>95</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1204,50 +1249,50 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>302</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E19" t="s">
         <v>95</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
-        <v>401</v>
+      <c r="B20">
+        <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
         <v>95</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
-        <v>402</v>
+      <c r="B21">
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="D21" t="s">
         <v>91</v>
@@ -1256,7 +1301,7 @@
         <v>95</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1264,10 +1309,10 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>501</v>
+        <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="D22" t="s">
         <v>91</v>
@@ -1276,30 +1321,27 @@
         <v>95</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
-        <v>502</v>
+      <c r="B23">
+        <v>122</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E23" t="s">
         <v>95</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1307,19 +1349,22 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>503</v>
+        <v>201</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" t="s">
         <v>95</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1327,19 +1372,22 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>504</v>
+        <v>202</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
         <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1347,19 +1395,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>505</v>
+        <v>203</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26" t="s">
         <v>95</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1367,10 +1418,10 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>506</v>
+        <v>301</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
         <v>92</v>
@@ -1379,7 +1430,7 @@
         <v>95</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1387,59 +1438,59 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>507</v>
+        <v>302</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E28" t="s">
         <v>95</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29">
-        <v>508</v>
+      <c r="B29" s="3">
+        <v>401</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E29" t="s">
         <v>95</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>509</v>
+      <c r="B30" s="3">
+        <v>402</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E30" t="s">
         <v>95</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1447,30 +1498,33 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>601</v>
+        <v>501</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E31" t="s">
         <v>95</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32">
-        <v>602</v>
+      <c r="B32" s="3">
+        <v>502</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s">
         <v>92</v>
@@ -1479,7 +1533,7 @@
         <v>95</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1487,10 +1541,10 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>603</v>
+        <v>503</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D33" t="s">
         <v>92</v>
@@ -1499,7 +1553,7 @@
         <v>95</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1507,10 +1561,10 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>604</v>
+        <v>504</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D34" t="s">
         <v>92</v>
@@ -1519,7 +1573,7 @@
         <v>95</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1527,53 +1581,50 @@
         <v>34</v>
       </c>
       <c r="B35" s="3">
-        <v>605</v>
+        <v>505</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E35" t="s">
         <v>95</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="3">
-        <v>606</v>
+      <c r="B36">
+        <v>506</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E36" t="s">
         <v>95</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="3">
-        <v>607</v>
+      <c r="B37">
+        <v>507</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
         <v>91</v>
@@ -1582,21 +1633,18 @@
         <v>95</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="3">
-        <v>608</v>
+      <c r="B38">
+        <v>508</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
         <v>91</v>
@@ -1605,18 +1653,18 @@
         <v>95</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="3">
-        <v>609</v>
+      <c r="B39">
+        <v>509</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D39" t="s">
         <v>92</v>
@@ -1625,18 +1673,18 @@
         <v>95</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="3">
-        <v>610</v>
+      <c r="B40">
+        <v>601</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
         <v>92</v>
@@ -1645,7 +1693,7 @@
         <v>95</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1653,42 +1701,39 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>701</v>
+        <v>602</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E41" t="s">
         <v>95</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="3">
-        <v>702</v>
+      <c r="B42">
+        <v>603</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E42" t="s">
         <v>95</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1696,90 +1741,96 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>703</v>
+        <v>604</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E43" t="s">
         <v>95</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44">
-        <v>704</v>
+      <c r="B44" s="3">
+        <v>605</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E44" t="s">
         <v>95</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45">
-        <v>705</v>
+      <c r="B45" s="3">
+        <v>606</v>
       </c>
       <c r="C45" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="D45" t="s">
         <v>91</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46">
-        <v>706</v>
+      <c r="B46" s="3">
+        <v>607</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D46" t="s">
         <v>91</v>
       </c>
       <c r="E46" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47">
-        <v>801</v>
+      <c r="B47" s="3">
+        <v>608</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D47" t="s">
         <v>91</v>
@@ -1788,31 +1839,27 @@
         <v>95</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48">
-        <v>802</v>
+      <c r="B48" s="3">
+        <v>609</v>
       </c>
       <c r="C48" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="D48" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E48" t="s">
-        <v>103</v>
-      </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1820,19 +1867,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="3">
-        <v>803</v>
+        <v>610</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E49" t="s">
-        <v>103</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1840,39 +1887,42 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>804</v>
+        <v>701</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E50" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51">
-        <v>804</v>
+      <c r="B51" s="3">
+        <v>702</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D51" t="s">
         <v>91</v>
       </c>
       <c r="E51" t="s">
-        <v>103</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1880,19 +1930,19 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>805</v>
+        <v>703</v>
       </c>
       <c r="C52" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D52" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E52" t="s">
         <v>95</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1900,19 +1950,19 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>901</v>
+        <v>704</v>
       </c>
       <c r="C53" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="D53" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E53" t="s">
-        <v>103</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1920,22 +1970,19 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>902</v>
+        <v>705</v>
       </c>
       <c r="C54" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D54" t="s">
         <v>91</v>
       </c>
       <c r="E54" t="s">
-        <v>95</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1943,21 +1990,208 @@
         <v>54</v>
       </c>
       <c r="B55">
+        <v>706</v>
+      </c>
+      <c r="C55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" t="s">
+        <v>103</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>801</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" t="s">
+        <v>91</v>
+      </c>
+      <c r="E56" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>802</v>
+      </c>
+      <c r="C57" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" t="s">
+        <v>91</v>
+      </c>
+      <c r="E57" t="s">
+        <v>103</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3">
+        <v>803</v>
+      </c>
+      <c r="C58" t="s">
+        <v>102</v>
+      </c>
+      <c r="D58" t="s">
+        <v>91</v>
+      </c>
+      <c r="E58" t="s">
+        <v>103</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>804</v>
+      </c>
+      <c r="C59" t="s">
+        <v>101</v>
+      </c>
+      <c r="D59" t="s">
+        <v>92</v>
+      </c>
+      <c r="E59" t="s">
+        <v>103</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>804</v>
+      </c>
+      <c r="C60" t="s">
+        <v>100</v>
+      </c>
+      <c r="D60" t="s">
+        <v>91</v>
+      </c>
+      <c r="E60" t="s">
+        <v>103</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>805</v>
+      </c>
+      <c r="C61" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" t="s">
+        <v>92</v>
+      </c>
+      <c r="E61" t="s">
+        <v>95</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>901</v>
+      </c>
+      <c r="C62" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" t="s">
+        <v>103</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>902</v>
+      </c>
+      <c r="C63" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" t="s">
+        <v>91</v>
+      </c>
+      <c r="E63" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
         <v>903</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C64" t="s">
         <v>34</v>
       </c>
-      <c r="D55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E55" t="s">
-        <v>95</v>
-      </c>
-      <c r="F55" s="1" t="s">
+      <c r="D64" t="s">
+        <v>91</v>
+      </c>
+      <c r="E64" t="s">
+        <v>95</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G64" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1967,67 +2201,67 @@
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G55">
-    <sortCondition ref="B1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G64">
+    <sortCondition ref="B38"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F17" r:id="rId1" xr:uid="{E26AB3C4-29AE-204B-97A1-8F7175E3530D}"/>
-    <hyperlink ref="F22" r:id="rId2" xr:uid="{20C7D150-9462-1F41-AAB7-2A899F9C969A}"/>
+    <hyperlink ref="F26" r:id="rId1" xr:uid="{E26AB3C4-29AE-204B-97A1-8F7175E3530D}"/>
+    <hyperlink ref="F31" r:id="rId2" xr:uid="{20C7D150-9462-1F41-AAB7-2A899F9C969A}"/>
     <hyperlink ref="F6" r:id="rId3" xr:uid="{62DFB431-E49A-4741-B60E-DA27CFC68C72}"/>
-    <hyperlink ref="F23" r:id="rId4" xr:uid="{8506591B-A62F-6948-8F5E-FAB4DE06D345}"/>
-    <hyperlink ref="F28" r:id="rId5" xr:uid="{7B4333D3-C25D-3144-87C0-B86DA456F7A0}"/>
-    <hyperlink ref="F29" r:id="rId6" xr:uid="{6F8B3503-4C3A-DC40-8109-C9D396669308}"/>
-    <hyperlink ref="F15" r:id="rId7" xr:uid="{E11F3A2B-4236-C240-B3A5-B3577F908F63}"/>
-    <hyperlink ref="F31" r:id="rId8" xr:uid="{208F8125-58C4-4848-9C44-457B5CA9C713}"/>
-    <hyperlink ref="F36" r:id="rId9" xr:uid="{3F4F2A3A-2C07-1A42-AC3D-471388B48825}"/>
-    <hyperlink ref="F37" r:id="rId10" xr:uid="{119BF651-F8C7-C24B-BA6B-34B978975A37}"/>
-    <hyperlink ref="F41" r:id="rId11" xr:uid="{2CCAB83E-F41F-B24B-90B4-A0DB21E63EAC}"/>
-    <hyperlink ref="F47" r:id="rId12" xr:uid="{0826D0C0-8E81-C044-9D15-BC27CA346E4D}"/>
-    <hyperlink ref="F40" r:id="rId13" xr:uid="{4DDE0179-60BD-8D4F-9D6C-2A707E2A6ABF}"/>
-    <hyperlink ref="F16" r:id="rId14" xr:uid="{0317F90B-9CF5-D440-98C2-9DD3D8CD4360}"/>
-    <hyperlink ref="F34" r:id="rId15" xr:uid="{B0FDC84E-194C-CA4A-B974-8821AB0DA033}"/>
-    <hyperlink ref="F27" r:id="rId16" xr:uid="{5C69EB99-4BB2-6C40-B120-40DC6CEA8E3D}"/>
+    <hyperlink ref="F32" r:id="rId4" xr:uid="{8506591B-A62F-6948-8F5E-FAB4DE06D345}"/>
+    <hyperlink ref="F37" r:id="rId5" xr:uid="{7B4333D3-C25D-3144-87C0-B86DA456F7A0}"/>
+    <hyperlink ref="F38" r:id="rId6" xr:uid="{6F8B3503-4C3A-DC40-8109-C9D396669308}"/>
+    <hyperlink ref="F24" r:id="rId7" xr:uid="{E11F3A2B-4236-C240-B3A5-B3577F908F63}"/>
+    <hyperlink ref="F40" r:id="rId8" xr:uid="{208F8125-58C4-4848-9C44-457B5CA9C713}"/>
+    <hyperlink ref="F45" r:id="rId9" xr:uid="{3F4F2A3A-2C07-1A42-AC3D-471388B48825}"/>
+    <hyperlink ref="F46" r:id="rId10" xr:uid="{119BF651-F8C7-C24B-BA6B-34B978975A37}"/>
+    <hyperlink ref="F50" r:id="rId11" xr:uid="{2CCAB83E-F41F-B24B-90B4-A0DB21E63EAC}"/>
+    <hyperlink ref="F56" r:id="rId12" xr:uid="{0826D0C0-8E81-C044-9D15-BC27CA346E4D}"/>
+    <hyperlink ref="F49" r:id="rId13" xr:uid="{4DDE0179-60BD-8D4F-9D6C-2A707E2A6ABF}"/>
+    <hyperlink ref="F25" r:id="rId14" xr:uid="{0317F90B-9CF5-D440-98C2-9DD3D8CD4360}"/>
+    <hyperlink ref="F43" r:id="rId15" xr:uid="{B0FDC84E-194C-CA4A-B974-8821AB0DA033}"/>
+    <hyperlink ref="F36" r:id="rId16" xr:uid="{5C69EB99-4BB2-6C40-B120-40DC6CEA8E3D}"/>
     <hyperlink ref="F2" r:id="rId17" xr:uid="{F9CDDCEB-59CD-AE47-A149-9CC74B550FEC}"/>
     <hyperlink ref="F3" r:id="rId18" xr:uid="{DE3B3CAA-EE98-3047-8B1C-3EEDFEAD7F28}"/>
     <hyperlink ref="F4" r:id="rId19" xr:uid="{3C4A7730-5B0F-F648-B13F-492DD0C989D9}"/>
-    <hyperlink ref="F26" r:id="rId20" xr:uid="{C1E695B0-BCA2-C543-ACE5-568C9F0303B1}"/>
-    <hyperlink ref="F38" r:id="rId21" xr:uid="{69EB5850-A79D-2249-8859-15359590B6A7}"/>
-    <hyperlink ref="F33" r:id="rId22" xr:uid="{C61A74F0-4B76-0C4E-BB52-AC63D005FD62}"/>
-    <hyperlink ref="F32" r:id="rId23" xr:uid="{81A92251-C09C-E44E-9A36-C9FE15E5FCD8}"/>
-    <hyperlink ref="F39" r:id="rId24" xr:uid="{F4F55930-9ED7-EA4F-BCBD-BCFEE7610B82}"/>
-    <hyperlink ref="F30" r:id="rId25" xr:uid="{0091B4FD-E7C4-1B4D-9203-8698BC24D565}"/>
-    <hyperlink ref="F42" r:id="rId26" xr:uid="{EB6B87D1-21E1-FC4E-B405-2E1E5231BF06}"/>
-    <hyperlink ref="F20" r:id="rId27" xr:uid="{71F90D41-9C86-E340-936E-3BB9C8F90010}"/>
-    <hyperlink ref="F24" r:id="rId28" xr:uid="{3DB60B42-7507-6C4E-BDAE-4CFDF2EB9C4B}"/>
-    <hyperlink ref="F35" r:id="rId29" xr:uid="{DE0DD6CB-D570-6945-B428-B9331B5F7EBD}"/>
-    <hyperlink ref="F25" r:id="rId30" xr:uid="{FEFB8575-764E-9449-AA25-D9D9E8089739}"/>
-    <hyperlink ref="F18" r:id="rId31" xr:uid="{D26F3756-D827-C34C-94BF-A5B4EB60366B}"/>
-    <hyperlink ref="F19" r:id="rId32" xr:uid="{784A9FC5-FAB0-B844-BE6A-3AF588A130C9}"/>
-    <hyperlink ref="F52" r:id="rId33" xr:uid="{EB6D586F-57BF-DD4A-8A35-36111ACF2E34}"/>
-    <hyperlink ref="F54" r:id="rId34" xr:uid="{4FE78F82-E051-BD41-AF8D-290EBCE2FD87}"/>
-    <hyperlink ref="F55" r:id="rId35" xr:uid="{EFC9C5A7-AB7E-6445-B238-3F6B90ECD054}"/>
-    <hyperlink ref="F43" r:id="rId36" xr:uid="{63617CDE-2E2D-AD4B-A08D-0848E898DD47}"/>
-    <hyperlink ref="F44" r:id="rId37" xr:uid="{3F4D27CA-6390-D84B-B25B-184101CE06FA}"/>
-    <hyperlink ref="G17" r:id="rId38" xr:uid="{07E7E11C-8841-7748-BFFF-540D5BB62B39}"/>
-    <hyperlink ref="G22" r:id="rId39" xr:uid="{41C80DDC-B435-E44A-B9FF-4AF4DE2F5656}"/>
-    <hyperlink ref="G15" r:id="rId40" xr:uid="{9F0DCD01-87D0-6A40-AE3F-32FC101B7188}"/>
-    <hyperlink ref="G36" r:id="rId41" xr:uid="{197BB746-FF15-2148-98BE-5BB0F1F85567}"/>
-    <hyperlink ref="G37" r:id="rId42" xr:uid="{C77A6773-BBA6-584C-8DAC-DE08233409B2}"/>
-    <hyperlink ref="G41" r:id="rId43" xr:uid="{7FC8D046-4E44-AD48-B3AC-C616091F1C3A}"/>
-    <hyperlink ref="G47" r:id="rId44" xr:uid="{F25E562D-AAF9-4041-B937-A59BAFE18EC5}"/>
-    <hyperlink ref="G16" r:id="rId45" xr:uid="{B3DC7E65-8B74-914F-93A8-6005B22982A3}"/>
+    <hyperlink ref="F35" r:id="rId20" xr:uid="{C1E695B0-BCA2-C543-ACE5-568C9F0303B1}"/>
+    <hyperlink ref="F47" r:id="rId21" xr:uid="{69EB5850-A79D-2249-8859-15359590B6A7}"/>
+    <hyperlink ref="F42" r:id="rId22" xr:uid="{C61A74F0-4B76-0C4E-BB52-AC63D005FD62}"/>
+    <hyperlink ref="F41" r:id="rId23" xr:uid="{81A92251-C09C-E44E-9A36-C9FE15E5FCD8}"/>
+    <hyperlink ref="F48" r:id="rId24" xr:uid="{F4F55930-9ED7-EA4F-BCBD-BCFEE7610B82}"/>
+    <hyperlink ref="F39" r:id="rId25" xr:uid="{0091B4FD-E7C4-1B4D-9203-8698BC24D565}"/>
+    <hyperlink ref="F51" r:id="rId26" xr:uid="{EB6B87D1-21E1-FC4E-B405-2E1E5231BF06}"/>
+    <hyperlink ref="F29" r:id="rId27" xr:uid="{71F90D41-9C86-E340-936E-3BB9C8F90010}"/>
+    <hyperlink ref="F33" r:id="rId28" xr:uid="{3DB60B42-7507-6C4E-BDAE-4CFDF2EB9C4B}"/>
+    <hyperlink ref="F44" r:id="rId29" xr:uid="{DE0DD6CB-D570-6945-B428-B9331B5F7EBD}"/>
+    <hyperlink ref="F34" r:id="rId30" xr:uid="{FEFB8575-764E-9449-AA25-D9D9E8089739}"/>
+    <hyperlink ref="F27" r:id="rId31" xr:uid="{D26F3756-D827-C34C-94BF-A5B4EB60366B}"/>
+    <hyperlink ref="F28" r:id="rId32" xr:uid="{784A9FC5-FAB0-B844-BE6A-3AF588A130C9}"/>
+    <hyperlink ref="F61" r:id="rId33" xr:uid="{EB6D586F-57BF-DD4A-8A35-36111ACF2E34}"/>
+    <hyperlink ref="F63" r:id="rId34" xr:uid="{4FE78F82-E051-BD41-AF8D-290EBCE2FD87}"/>
+    <hyperlink ref="F64" r:id="rId35" xr:uid="{EFC9C5A7-AB7E-6445-B238-3F6B90ECD054}"/>
+    <hyperlink ref="F52" r:id="rId36" xr:uid="{63617CDE-2E2D-AD4B-A08D-0848E898DD47}"/>
+    <hyperlink ref="F53" r:id="rId37" xr:uid="{3F4D27CA-6390-D84B-B25B-184101CE06FA}"/>
+    <hyperlink ref="G26" r:id="rId38" xr:uid="{07E7E11C-8841-7748-BFFF-540D5BB62B39}"/>
+    <hyperlink ref="G31" r:id="rId39" xr:uid="{41C80DDC-B435-E44A-B9FF-4AF4DE2F5656}"/>
+    <hyperlink ref="G24" r:id="rId40" xr:uid="{9F0DCD01-87D0-6A40-AE3F-32FC101B7188}"/>
+    <hyperlink ref="G45" r:id="rId41" xr:uid="{197BB746-FF15-2148-98BE-5BB0F1F85567}"/>
+    <hyperlink ref="G46" r:id="rId42" xr:uid="{C77A6773-BBA6-584C-8DAC-DE08233409B2}"/>
+    <hyperlink ref="G50" r:id="rId43" xr:uid="{7FC8D046-4E44-AD48-B3AC-C616091F1C3A}"/>
+    <hyperlink ref="G56" r:id="rId44" xr:uid="{F25E562D-AAF9-4041-B937-A59BAFE18EC5}"/>
+    <hyperlink ref="G25" r:id="rId45" xr:uid="{B3DC7E65-8B74-914F-93A8-6005B22982A3}"/>
     <hyperlink ref="G2" r:id="rId46" xr:uid="{843CA431-F6E9-1B4D-845E-601D7EDB0BB1}"/>
     <hyperlink ref="G3" r:id="rId47" xr:uid="{4D5CA3E4-8FD4-DE4A-83B2-0E8DDA142970}"/>
     <hyperlink ref="G4" r:id="rId48" xr:uid="{F45701A4-E062-F544-AEFE-3543E8569B6E}"/>
-    <hyperlink ref="G54" r:id="rId49" xr:uid="{985334CD-1972-8442-AD5A-14F3D57E92CF}"/>
-    <hyperlink ref="G55" r:id="rId50" xr:uid="{5556EC84-5DAB-B246-9C73-76642D572382}"/>
-    <hyperlink ref="G53" r:id="rId51" xr:uid="{51C1EF83-209F-024C-B3DA-10B36D1E5A4C}"/>
-    <hyperlink ref="G46" r:id="rId52" xr:uid="{BED6B18A-333C-D348-9DA2-FBE4265E3C32}"/>
-    <hyperlink ref="G45" r:id="rId53" xr:uid="{68C79AD3-9ED9-684B-BA88-B3D3EE552B52}"/>
-    <hyperlink ref="G51" r:id="rId54" xr:uid="{149FC972-472B-6F48-BC30-B43708381DDC}"/>
-    <hyperlink ref="G50" r:id="rId55" xr:uid="{6E323EF5-0E5A-5B4C-BD17-16A6D0E2C053}"/>
-    <hyperlink ref="G49" r:id="rId56" xr:uid="{96FE3BD0-D39E-7A4F-953E-7831D516D31B}"/>
-    <hyperlink ref="F21" r:id="rId57" xr:uid="{D6022A27-41D7-5246-8EF9-8E2A4D9AC1A6}"/>
+    <hyperlink ref="G63" r:id="rId49" xr:uid="{985334CD-1972-8442-AD5A-14F3D57E92CF}"/>
+    <hyperlink ref="G64" r:id="rId50" xr:uid="{5556EC84-5DAB-B246-9C73-76642D572382}"/>
+    <hyperlink ref="G62" r:id="rId51" xr:uid="{51C1EF83-209F-024C-B3DA-10B36D1E5A4C}"/>
+    <hyperlink ref="G55" r:id="rId52" xr:uid="{BED6B18A-333C-D348-9DA2-FBE4265E3C32}"/>
+    <hyperlink ref="G54" r:id="rId53" xr:uid="{68C79AD3-9ED9-684B-BA88-B3D3EE552B52}"/>
+    <hyperlink ref="G60" r:id="rId54" xr:uid="{149FC972-472B-6F48-BC30-B43708381DDC}"/>
+    <hyperlink ref="G59" r:id="rId55" xr:uid="{6E323EF5-0E5A-5B4C-BD17-16A6D0E2C053}"/>
+    <hyperlink ref="G58" r:id="rId56" xr:uid="{96FE3BD0-D39E-7A4F-953E-7831D516D31B}"/>
+    <hyperlink ref="F30" r:id="rId57" xr:uid="{D6022A27-41D7-5246-8EF9-8E2A4D9AC1A6}"/>
     <hyperlink ref="F5" r:id="rId58" xr:uid="{532705D3-72B5-C54F-B311-5B790A4C8170}"/>
     <hyperlink ref="F10" r:id="rId59" xr:uid="{07F89B1F-6BF6-EC45-84D1-D16AABC8DE2F}"/>
     <hyperlink ref="F9" r:id="rId60" xr:uid="{E2D8DF9F-F502-0243-964F-5B6E3821EB45}"/>
@@ -2037,6 +2271,15 @@
     <hyperlink ref="F11" r:id="rId64" xr:uid="{2D057E9E-BED0-6E4D-85F7-7DF9AF7C772D}"/>
     <hyperlink ref="F13" r:id="rId65" xr:uid="{5338C8C7-0F3B-2447-83CB-A823FB7FA683}"/>
     <hyperlink ref="F14" r:id="rId66" xr:uid="{C413640A-E27E-E24B-B726-4D512D306CE4}"/>
+    <hyperlink ref="F15" r:id="rId67" xr:uid="{D17F65B7-496F-314C-A553-2CF986AEBFA8}"/>
+    <hyperlink ref="F16" r:id="rId68" xr:uid="{09C9E7A7-37B4-A441-97F2-172555E88642}"/>
+    <hyperlink ref="F17" r:id="rId69" xr:uid="{A087CE46-66E3-C94A-94D2-FA762CC2EAC4}"/>
+    <hyperlink ref="F18" r:id="rId70" xr:uid="{9EA404A2-1F3E-9C42-AAEC-66ED758408D4}"/>
+    <hyperlink ref="F19" r:id="rId71" xr:uid="{D46ECBFC-2956-D141-944A-DBFBBB02AC76}"/>
+    <hyperlink ref="F20" r:id="rId72" xr:uid="{BBFF3588-BBB3-A146-9AEB-E97A22E00C49}"/>
+    <hyperlink ref="F21" r:id="rId73" xr:uid="{70B7B8F1-56CE-794A-A9C4-C40691F210B1}"/>
+    <hyperlink ref="F22" r:id="rId74" xr:uid="{C3E16E28-AFF0-AE43-AE16-B4A0593FDA96}"/>
+    <hyperlink ref="F23" r:id="rId75" xr:uid="{198162A4-B86B-E649-B65E-10474D73EDE3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new project entries
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/likarajo/#GITHUB/Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/likarajo/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F51651A-0FEC-AE4B-8AD9-B487D633EDB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5315C49-D68F-0D40-BA96-0C17664223C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="460" windowWidth="26260" windowHeight="16660" xr2:uid="{26E92A9D-7BD1-914F-959E-FC63F09E2183}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$60</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="163">
   <si>
     <t>website</t>
   </si>
@@ -487,6 +487,42 @@
   </si>
   <si>
     <t>weather_predcition</t>
+  </si>
+  <si>
+    <t>covid19sentiments</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/covid19Sentiments</t>
+  </si>
+  <si>
+    <t>https://likarajo.github.io/covid19Sentiments</t>
+  </si>
+  <si>
+    <t>covid19</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/covid19</t>
+  </si>
+  <si>
+    <t>https://likarajo.github.io/covid19</t>
+  </si>
+  <si>
+    <t>digit_recognition</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/digit_recognition</t>
+  </si>
+  <si>
+    <t>image_recognition</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/image_recognition</t>
+  </si>
+  <si>
+    <t>instacart_analysis</t>
+  </si>
+  <si>
+    <t>https://github.com/likarajo/instacart_analysis</t>
   </si>
 </sst>
 </file>
@@ -857,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2CE227-055B-2D42-8D36-FD50B0BC9862}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1349,10 +1385,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>201</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="D24" t="s">
         <v>91</v>
@@ -1361,10 +1397,10 @@
         <v>95</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1372,10 +1408,10 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>202</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>154</v>
       </c>
       <c r="D25" t="s">
         <v>91</v>
@@ -1384,44 +1420,42 @@
         <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
-        <v>203</v>
+      <c r="B26">
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
         <v>95</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>301</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="D27" t="s">
         <v>92</v>
@@ -1430,18 +1464,19 @@
         <v>95</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>302</v>
+        <v>127</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>161</v>
       </c>
       <c r="D28" t="s">
         <v>92</v>
@@ -1450,38 +1485,42 @@
         <v>95</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
-        <v>401</v>
+      <c r="B29">
+        <v>201</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E29" t="s">
         <v>95</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>66</v>
+        <v>46</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
-        <v>402</v>
+      <c r="B30">
+        <v>202</v>
       </c>
       <c r="C30" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
         <v>91</v>
@@ -1490,18 +1529,21 @@
         <v>95</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>114</v>
+        <v>53</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31">
-        <v>501</v>
+      <c r="B31" s="3">
+        <v>203</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>91</v>
@@ -1510,21 +1552,21 @@
         <v>95</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
-        <v>502</v>
+      <c r="B32">
+        <v>301</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
         <v>92</v>
@@ -1533,7 +1575,7 @@
         <v>95</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1541,10 +1583,10 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>503</v>
+        <v>302</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
         <v>92</v>
@@ -1553,18 +1595,18 @@
         <v>95</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>504</v>
+      <c r="B34" s="3">
+        <v>401</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
         <v>92</v>
@@ -1573,7 +1615,7 @@
         <v>95</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1581,19 +1623,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="3">
-        <v>505</v>
+        <v>402</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E35" t="s">
         <v>95</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1601,39 +1643,42 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E36" t="s">
         <v>95</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37">
-        <v>507</v>
+      <c r="B37" s="3">
+        <v>502</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E37" t="s">
         <v>95</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1641,19 +1686,19 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E38" t="s">
         <v>95</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1661,10 +1706,10 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D39" t="s">
         <v>92</v>
@@ -1673,18 +1718,18 @@
         <v>95</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40">
-        <v>601</v>
+      <c r="B40" s="3">
+        <v>505</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D40" t="s">
         <v>92</v>
@@ -1693,7 +1738,7 @@
         <v>95</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1701,10 +1746,10 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>602</v>
+        <v>506</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
         <v>92</v>
@@ -1713,7 +1758,7 @@
         <v>95</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1721,19 +1766,19 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>603</v>
+        <v>507</v>
       </c>
       <c r="C42" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E42" t="s">
         <v>95</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1741,116 +1786,110 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>604</v>
+        <v>508</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E43" t="s">
         <v>95</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="3">
-        <v>605</v>
+      <c r="B44">
+        <v>509</v>
       </c>
       <c r="C44" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E44" t="s">
         <v>95</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="3">
-        <v>606</v>
+      <c r="B45">
+        <v>601</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E45" t="s">
         <v>95</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="3">
-        <v>607</v>
+      <c r="B46">
+        <v>602</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E46" t="s">
         <v>95</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="3">
-        <v>608</v>
+      <c r="B47">
+        <v>603</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E47" t="s">
         <v>95</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="3">
-        <v>609</v>
+      <c r="B48">
+        <v>604</v>
       </c>
       <c r="C48" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D48" t="s">
         <v>92</v>
@@ -1859,7 +1898,7 @@
         <v>95</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1867,30 +1906,30 @@
         <v>48</v>
       </c>
       <c r="B49" s="3">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E49" t="s">
         <v>95</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50">
-        <v>701</v>
+      <c r="B50" s="3">
+        <v>606</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
         <v>91</v>
@@ -1899,10 +1938,10 @@
         <v>95</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1910,10 +1949,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="3">
-        <v>702</v>
+        <v>607</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D51" t="s">
         <v>91</v>
@@ -1922,67 +1961,70 @@
         <v>95</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52">
-        <v>703</v>
+      <c r="B52" s="3">
+        <v>608</v>
       </c>
       <c r="C52" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E52" t="s">
         <v>95</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53">
-        <v>704</v>
+      <c r="B53" s="3">
+        <v>609</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E53" t="s">
         <v>95</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54">
-        <v>705</v>
+      <c r="B54" s="3">
+        <v>610</v>
       </c>
       <c r="C54" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E54" t="s">
-        <v>103</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1990,30 +2032,33 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="C55" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="D55" t="s">
         <v>91</v>
       </c>
       <c r="E55" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56">
-        <v>801</v>
+      <c r="B56" s="3">
+        <v>702</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D56" t="s">
         <v>91</v>
@@ -2022,10 +2067,7 @@
         <v>95</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -2033,40 +2075,39 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>802</v>
+        <v>703</v>
       </c>
       <c r="C57" t="s">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="D57" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E57" t="s">
-        <v>103</v>
-      </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="3">
-        <v>803</v>
+      <c r="B58">
+        <v>704</v>
       </c>
       <c r="C58" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="D58" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E58" t="s">
-        <v>103</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -2074,19 +2115,19 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>804</v>
+        <v>705</v>
       </c>
       <c r="C59" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E59" t="s">
         <v>103</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -2094,10 +2135,10 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>804</v>
+        <v>706</v>
       </c>
       <c r="C60" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D60" t="s">
         <v>91</v>
@@ -2106,7 +2147,7 @@
         <v>103</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -2114,19 +2155,22 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="C61" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E61" t="s">
         <v>95</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -2134,10 +2178,10 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>901</v>
+        <v>802</v>
       </c>
       <c r="C62" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="D62" t="s">
         <v>91</v>
@@ -2145,31 +2189,29 @@
       <c r="E62" t="s">
         <v>103</v>
       </c>
+      <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63">
-        <v>902</v>
+      <c r="B63" s="3">
+        <v>803</v>
       </c>
       <c r="C63" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="D63" t="s">
         <v>91</v>
       </c>
       <c r="E63" t="s">
-        <v>95</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -2177,91 +2219,194 @@
         <v>63</v>
       </c>
       <c r="B64">
+        <v>804</v>
+      </c>
+      <c r="C64" t="s">
+        <v>101</v>
+      </c>
+      <c r="D64" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" t="s">
+        <v>103</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>804</v>
+      </c>
+      <c r="C65" t="s">
+        <v>100</v>
+      </c>
+      <c r="D65" t="s">
+        <v>91</v>
+      </c>
+      <c r="E65" t="s">
+        <v>103</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>805</v>
+      </c>
+      <c r="C66" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E66" t="s">
+        <v>95</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>901</v>
+      </c>
+      <c r="C67" t="s">
+        <v>97</v>
+      </c>
+      <c r="D67" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>902</v>
+      </c>
+      <c r="C68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" t="s">
+        <v>91</v>
+      </c>
+      <c r="E68" t="s">
+        <v>95</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
         <v>903</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C69" t="s">
         <v>34</v>
       </c>
-      <c r="D64" t="s">
-        <v>91</v>
-      </c>
-      <c r="E64" t="s">
-        <v>95</v>
-      </c>
-      <c r="F64" s="1" t="s">
+      <c r="D69" t="s">
+        <v>91</v>
+      </c>
+      <c r="E69" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G55" xr:uid="{27AC6761-2437-C441-907E-B1FB733C8BAA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G55">
+  <autoFilter ref="B1:G60" xr:uid="{27AC6761-2437-C441-907E-B1FB733C8BAA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G60">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G64">
-    <sortCondition ref="B38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G69">
+    <sortCondition ref="B43"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F26" r:id="rId1" xr:uid="{E26AB3C4-29AE-204B-97A1-8F7175E3530D}"/>
-    <hyperlink ref="F31" r:id="rId2" xr:uid="{20C7D150-9462-1F41-AAB7-2A899F9C969A}"/>
+    <hyperlink ref="F31" r:id="rId1" xr:uid="{E26AB3C4-29AE-204B-97A1-8F7175E3530D}"/>
+    <hyperlink ref="F36" r:id="rId2" xr:uid="{20C7D150-9462-1F41-AAB7-2A899F9C969A}"/>
     <hyperlink ref="F6" r:id="rId3" xr:uid="{62DFB431-E49A-4741-B60E-DA27CFC68C72}"/>
-    <hyperlink ref="F32" r:id="rId4" xr:uid="{8506591B-A62F-6948-8F5E-FAB4DE06D345}"/>
-    <hyperlink ref="F37" r:id="rId5" xr:uid="{7B4333D3-C25D-3144-87C0-B86DA456F7A0}"/>
-    <hyperlink ref="F38" r:id="rId6" xr:uid="{6F8B3503-4C3A-DC40-8109-C9D396669308}"/>
-    <hyperlink ref="F24" r:id="rId7" xr:uid="{E11F3A2B-4236-C240-B3A5-B3577F908F63}"/>
-    <hyperlink ref="F40" r:id="rId8" xr:uid="{208F8125-58C4-4848-9C44-457B5CA9C713}"/>
-    <hyperlink ref="F45" r:id="rId9" xr:uid="{3F4F2A3A-2C07-1A42-AC3D-471388B48825}"/>
-    <hyperlink ref="F46" r:id="rId10" xr:uid="{119BF651-F8C7-C24B-BA6B-34B978975A37}"/>
-    <hyperlink ref="F50" r:id="rId11" xr:uid="{2CCAB83E-F41F-B24B-90B4-A0DB21E63EAC}"/>
-    <hyperlink ref="F56" r:id="rId12" xr:uid="{0826D0C0-8E81-C044-9D15-BC27CA346E4D}"/>
-    <hyperlink ref="F49" r:id="rId13" xr:uid="{4DDE0179-60BD-8D4F-9D6C-2A707E2A6ABF}"/>
-    <hyperlink ref="F25" r:id="rId14" xr:uid="{0317F90B-9CF5-D440-98C2-9DD3D8CD4360}"/>
-    <hyperlink ref="F43" r:id="rId15" xr:uid="{B0FDC84E-194C-CA4A-B974-8821AB0DA033}"/>
-    <hyperlink ref="F36" r:id="rId16" xr:uid="{5C69EB99-4BB2-6C40-B120-40DC6CEA8E3D}"/>
+    <hyperlink ref="F37" r:id="rId4" xr:uid="{8506591B-A62F-6948-8F5E-FAB4DE06D345}"/>
+    <hyperlink ref="F42" r:id="rId5" xr:uid="{7B4333D3-C25D-3144-87C0-B86DA456F7A0}"/>
+    <hyperlink ref="F43" r:id="rId6" xr:uid="{6F8B3503-4C3A-DC40-8109-C9D396669308}"/>
+    <hyperlink ref="F29" r:id="rId7" xr:uid="{E11F3A2B-4236-C240-B3A5-B3577F908F63}"/>
+    <hyperlink ref="F45" r:id="rId8" xr:uid="{208F8125-58C4-4848-9C44-457B5CA9C713}"/>
+    <hyperlink ref="F50" r:id="rId9" xr:uid="{3F4F2A3A-2C07-1A42-AC3D-471388B48825}"/>
+    <hyperlink ref="F51" r:id="rId10" xr:uid="{119BF651-F8C7-C24B-BA6B-34B978975A37}"/>
+    <hyperlink ref="F55" r:id="rId11" xr:uid="{2CCAB83E-F41F-B24B-90B4-A0DB21E63EAC}"/>
+    <hyperlink ref="F61" r:id="rId12" xr:uid="{0826D0C0-8E81-C044-9D15-BC27CA346E4D}"/>
+    <hyperlink ref="F54" r:id="rId13" xr:uid="{4DDE0179-60BD-8D4F-9D6C-2A707E2A6ABF}"/>
+    <hyperlink ref="F30" r:id="rId14" xr:uid="{0317F90B-9CF5-D440-98C2-9DD3D8CD4360}"/>
+    <hyperlink ref="F48" r:id="rId15" xr:uid="{B0FDC84E-194C-CA4A-B974-8821AB0DA033}"/>
+    <hyperlink ref="F41" r:id="rId16" xr:uid="{5C69EB99-4BB2-6C40-B120-40DC6CEA8E3D}"/>
     <hyperlink ref="F2" r:id="rId17" xr:uid="{F9CDDCEB-59CD-AE47-A149-9CC74B550FEC}"/>
     <hyperlink ref="F3" r:id="rId18" xr:uid="{DE3B3CAA-EE98-3047-8B1C-3EEDFEAD7F28}"/>
     <hyperlink ref="F4" r:id="rId19" xr:uid="{3C4A7730-5B0F-F648-B13F-492DD0C989D9}"/>
-    <hyperlink ref="F35" r:id="rId20" xr:uid="{C1E695B0-BCA2-C543-ACE5-568C9F0303B1}"/>
-    <hyperlink ref="F47" r:id="rId21" xr:uid="{69EB5850-A79D-2249-8859-15359590B6A7}"/>
-    <hyperlink ref="F42" r:id="rId22" xr:uid="{C61A74F0-4B76-0C4E-BB52-AC63D005FD62}"/>
-    <hyperlink ref="F41" r:id="rId23" xr:uid="{81A92251-C09C-E44E-9A36-C9FE15E5FCD8}"/>
-    <hyperlink ref="F48" r:id="rId24" xr:uid="{F4F55930-9ED7-EA4F-BCBD-BCFEE7610B82}"/>
-    <hyperlink ref="F39" r:id="rId25" xr:uid="{0091B4FD-E7C4-1B4D-9203-8698BC24D565}"/>
-    <hyperlink ref="F51" r:id="rId26" xr:uid="{EB6B87D1-21E1-FC4E-B405-2E1E5231BF06}"/>
-    <hyperlink ref="F29" r:id="rId27" xr:uid="{71F90D41-9C86-E340-936E-3BB9C8F90010}"/>
-    <hyperlink ref="F33" r:id="rId28" xr:uid="{3DB60B42-7507-6C4E-BDAE-4CFDF2EB9C4B}"/>
-    <hyperlink ref="F44" r:id="rId29" xr:uid="{DE0DD6CB-D570-6945-B428-B9331B5F7EBD}"/>
-    <hyperlink ref="F34" r:id="rId30" xr:uid="{FEFB8575-764E-9449-AA25-D9D9E8089739}"/>
-    <hyperlink ref="F27" r:id="rId31" xr:uid="{D26F3756-D827-C34C-94BF-A5B4EB60366B}"/>
-    <hyperlink ref="F28" r:id="rId32" xr:uid="{784A9FC5-FAB0-B844-BE6A-3AF588A130C9}"/>
-    <hyperlink ref="F61" r:id="rId33" xr:uid="{EB6D586F-57BF-DD4A-8A35-36111ACF2E34}"/>
-    <hyperlink ref="F63" r:id="rId34" xr:uid="{4FE78F82-E051-BD41-AF8D-290EBCE2FD87}"/>
-    <hyperlink ref="F64" r:id="rId35" xr:uid="{EFC9C5A7-AB7E-6445-B238-3F6B90ECD054}"/>
-    <hyperlink ref="F52" r:id="rId36" xr:uid="{63617CDE-2E2D-AD4B-A08D-0848E898DD47}"/>
-    <hyperlink ref="F53" r:id="rId37" xr:uid="{3F4D27CA-6390-D84B-B25B-184101CE06FA}"/>
-    <hyperlink ref="G26" r:id="rId38" xr:uid="{07E7E11C-8841-7748-BFFF-540D5BB62B39}"/>
-    <hyperlink ref="G31" r:id="rId39" xr:uid="{41C80DDC-B435-E44A-B9FF-4AF4DE2F5656}"/>
-    <hyperlink ref="G24" r:id="rId40" xr:uid="{9F0DCD01-87D0-6A40-AE3F-32FC101B7188}"/>
-    <hyperlink ref="G45" r:id="rId41" xr:uid="{197BB746-FF15-2148-98BE-5BB0F1F85567}"/>
-    <hyperlink ref="G46" r:id="rId42" xr:uid="{C77A6773-BBA6-584C-8DAC-DE08233409B2}"/>
-    <hyperlink ref="G50" r:id="rId43" xr:uid="{7FC8D046-4E44-AD48-B3AC-C616091F1C3A}"/>
-    <hyperlink ref="G56" r:id="rId44" xr:uid="{F25E562D-AAF9-4041-B937-A59BAFE18EC5}"/>
-    <hyperlink ref="G25" r:id="rId45" xr:uid="{B3DC7E65-8B74-914F-93A8-6005B22982A3}"/>
+    <hyperlink ref="F40" r:id="rId20" xr:uid="{C1E695B0-BCA2-C543-ACE5-568C9F0303B1}"/>
+    <hyperlink ref="F52" r:id="rId21" xr:uid="{69EB5850-A79D-2249-8859-15359590B6A7}"/>
+    <hyperlink ref="F47" r:id="rId22" xr:uid="{C61A74F0-4B76-0C4E-BB52-AC63D005FD62}"/>
+    <hyperlink ref="F46" r:id="rId23" xr:uid="{81A92251-C09C-E44E-9A36-C9FE15E5FCD8}"/>
+    <hyperlink ref="F53" r:id="rId24" xr:uid="{F4F55930-9ED7-EA4F-BCBD-BCFEE7610B82}"/>
+    <hyperlink ref="F44" r:id="rId25" xr:uid="{0091B4FD-E7C4-1B4D-9203-8698BC24D565}"/>
+    <hyperlink ref="F56" r:id="rId26" xr:uid="{EB6B87D1-21E1-FC4E-B405-2E1E5231BF06}"/>
+    <hyperlink ref="F34" r:id="rId27" xr:uid="{71F90D41-9C86-E340-936E-3BB9C8F90010}"/>
+    <hyperlink ref="F38" r:id="rId28" xr:uid="{3DB60B42-7507-6C4E-BDAE-4CFDF2EB9C4B}"/>
+    <hyperlink ref="F49" r:id="rId29" xr:uid="{DE0DD6CB-D570-6945-B428-B9331B5F7EBD}"/>
+    <hyperlink ref="F39" r:id="rId30" xr:uid="{FEFB8575-764E-9449-AA25-D9D9E8089739}"/>
+    <hyperlink ref="F32" r:id="rId31" xr:uid="{D26F3756-D827-C34C-94BF-A5B4EB60366B}"/>
+    <hyperlink ref="F33" r:id="rId32" xr:uid="{784A9FC5-FAB0-B844-BE6A-3AF588A130C9}"/>
+    <hyperlink ref="F66" r:id="rId33" xr:uid="{EB6D586F-57BF-DD4A-8A35-36111ACF2E34}"/>
+    <hyperlink ref="F68" r:id="rId34" xr:uid="{4FE78F82-E051-BD41-AF8D-290EBCE2FD87}"/>
+    <hyperlink ref="F69" r:id="rId35" xr:uid="{EFC9C5A7-AB7E-6445-B238-3F6B90ECD054}"/>
+    <hyperlink ref="F57" r:id="rId36" xr:uid="{63617CDE-2E2D-AD4B-A08D-0848E898DD47}"/>
+    <hyperlink ref="F58" r:id="rId37" xr:uid="{3F4D27CA-6390-D84B-B25B-184101CE06FA}"/>
+    <hyperlink ref="G31" r:id="rId38" xr:uid="{07E7E11C-8841-7748-BFFF-540D5BB62B39}"/>
+    <hyperlink ref="G36" r:id="rId39" xr:uid="{41C80DDC-B435-E44A-B9FF-4AF4DE2F5656}"/>
+    <hyperlink ref="G29" r:id="rId40" xr:uid="{9F0DCD01-87D0-6A40-AE3F-32FC101B7188}"/>
+    <hyperlink ref="G50" r:id="rId41" xr:uid="{197BB746-FF15-2148-98BE-5BB0F1F85567}"/>
+    <hyperlink ref="G51" r:id="rId42" xr:uid="{C77A6773-BBA6-584C-8DAC-DE08233409B2}"/>
+    <hyperlink ref="G55" r:id="rId43" xr:uid="{7FC8D046-4E44-AD48-B3AC-C616091F1C3A}"/>
+    <hyperlink ref="G61" r:id="rId44" xr:uid="{F25E562D-AAF9-4041-B937-A59BAFE18EC5}"/>
+    <hyperlink ref="G30" r:id="rId45" xr:uid="{B3DC7E65-8B74-914F-93A8-6005B22982A3}"/>
     <hyperlink ref="G2" r:id="rId46" xr:uid="{843CA431-F6E9-1B4D-845E-601D7EDB0BB1}"/>
     <hyperlink ref="G3" r:id="rId47" xr:uid="{4D5CA3E4-8FD4-DE4A-83B2-0E8DDA142970}"/>
     <hyperlink ref="G4" r:id="rId48" xr:uid="{F45701A4-E062-F544-AEFE-3543E8569B6E}"/>
-    <hyperlink ref="G63" r:id="rId49" xr:uid="{985334CD-1972-8442-AD5A-14F3D57E92CF}"/>
-    <hyperlink ref="G64" r:id="rId50" xr:uid="{5556EC84-5DAB-B246-9C73-76642D572382}"/>
-    <hyperlink ref="G62" r:id="rId51" xr:uid="{51C1EF83-209F-024C-B3DA-10B36D1E5A4C}"/>
-    <hyperlink ref="G55" r:id="rId52" xr:uid="{BED6B18A-333C-D348-9DA2-FBE4265E3C32}"/>
-    <hyperlink ref="G54" r:id="rId53" xr:uid="{68C79AD3-9ED9-684B-BA88-B3D3EE552B52}"/>
-    <hyperlink ref="G60" r:id="rId54" xr:uid="{149FC972-472B-6F48-BC30-B43708381DDC}"/>
-    <hyperlink ref="G59" r:id="rId55" xr:uid="{6E323EF5-0E5A-5B4C-BD17-16A6D0E2C053}"/>
-    <hyperlink ref="G58" r:id="rId56" xr:uid="{96FE3BD0-D39E-7A4F-953E-7831D516D31B}"/>
-    <hyperlink ref="F30" r:id="rId57" xr:uid="{D6022A27-41D7-5246-8EF9-8E2A4D9AC1A6}"/>
+    <hyperlink ref="G68" r:id="rId49" xr:uid="{985334CD-1972-8442-AD5A-14F3D57E92CF}"/>
+    <hyperlink ref="G69" r:id="rId50" xr:uid="{5556EC84-5DAB-B246-9C73-76642D572382}"/>
+    <hyperlink ref="G67" r:id="rId51" xr:uid="{51C1EF83-209F-024C-B3DA-10B36D1E5A4C}"/>
+    <hyperlink ref="G60" r:id="rId52" xr:uid="{BED6B18A-333C-D348-9DA2-FBE4265E3C32}"/>
+    <hyperlink ref="G59" r:id="rId53" xr:uid="{68C79AD3-9ED9-684B-BA88-B3D3EE552B52}"/>
+    <hyperlink ref="G65" r:id="rId54" xr:uid="{149FC972-472B-6F48-BC30-B43708381DDC}"/>
+    <hyperlink ref="G64" r:id="rId55" xr:uid="{6E323EF5-0E5A-5B4C-BD17-16A6D0E2C053}"/>
+    <hyperlink ref="G63" r:id="rId56" xr:uid="{96FE3BD0-D39E-7A4F-953E-7831D516D31B}"/>
+    <hyperlink ref="F35" r:id="rId57" xr:uid="{D6022A27-41D7-5246-8EF9-8E2A4D9AC1A6}"/>
     <hyperlink ref="F5" r:id="rId58" xr:uid="{532705D3-72B5-C54F-B311-5B790A4C8170}"/>
     <hyperlink ref="F10" r:id="rId59" xr:uid="{07F89B1F-6BF6-EC45-84D1-D16AABC8DE2F}"/>
     <hyperlink ref="F9" r:id="rId60" xr:uid="{E2D8DF9F-F502-0243-964F-5B6E3821EB45}"/>
@@ -2280,6 +2425,13 @@
     <hyperlink ref="F21" r:id="rId73" xr:uid="{70B7B8F1-56CE-794A-A9C4-C40691F210B1}"/>
     <hyperlink ref="F22" r:id="rId74" xr:uid="{C3E16E28-AFF0-AE43-AE16-B4A0593FDA96}"/>
     <hyperlink ref="F23" r:id="rId75" xr:uid="{198162A4-B86B-E649-B65E-10474D73EDE3}"/>
+    <hyperlink ref="F24" r:id="rId76" xr:uid="{CAF8733F-450B-7D4B-95A9-9D7CFAA13541}"/>
+    <hyperlink ref="G24" r:id="rId77" xr:uid="{EE263171-DF13-D545-8E63-1FD306C10FB1}"/>
+    <hyperlink ref="F25" r:id="rId78" xr:uid="{5B40CF8C-58C5-2445-BE87-75CA4CE0F727}"/>
+    <hyperlink ref="G25" r:id="rId79" xr:uid="{0B2C9CE3-FB9A-AF40-AD4F-6CF2E3831CE3}"/>
+    <hyperlink ref="F27" r:id="rId80" xr:uid="{DF7D7515-A6AA-7A49-8D0B-31A26BC22901}"/>
+    <hyperlink ref="F26" r:id="rId81" xr:uid="{3FA3F5C7-23D3-8E4D-B5B6-71046038026B}"/>
+    <hyperlink ref="F28" r:id="rId82" xr:uid="{D0D6E152-3F37-CC4E-954B-1F80BD4FE9F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>